<commit_message>
new results of covid analisys work
modelling coefficients of lotka-Volterra differential equation aquired
</commit_message>
<xml_diff>
--- a/output_xlsx/metadata_conf.xlsx
+++ b/output_xlsx/metadata_conf.xlsx
@@ -1217,13 +1217,13 @@
         <v>67.709953</v>
       </c>
       <c r="D2" t="n">
-        <v>32175.1531728665</v>
+        <v>33923.2510288066</v>
       </c>
       <c r="E2" t="n">
-        <v>32175.1531728665</v>
+        <v>33923.2510288066</v>
       </c>
       <c r="F2" t="n">
-        <v>14704045</v>
+        <v>16486700</v>
       </c>
     </row>
     <row r="3">
@@ -1237,13 +1237,13 @@
         <v>20.1683</v>
       </c>
       <c r="D3" t="n">
-        <v>32601.4398249453</v>
+        <v>38499.8971193416</v>
       </c>
       <c r="E3" t="n">
-        <v>32601.4398249453</v>
+        <v>38499.8971193416</v>
       </c>
       <c r="F3" t="n">
-        <v>14898858</v>
+        <v>18710950</v>
       </c>
     </row>
     <row r="4">
@@ -1257,13 +1257,13 @@
         <v>1.6596</v>
       </c>
       <c r="D4" t="n">
-        <v>50506.2647702407</v>
+        <v>54864.512345679</v>
       </c>
       <c r="E4" t="n">
-        <v>50506.2647702407</v>
+        <v>54864.512345679</v>
       </c>
       <c r="F4" t="n">
-        <v>23081363</v>
+        <v>26664153</v>
       </c>
     </row>
     <row r="5">
@@ -1277,13 +1277,13 @@
         <v>1.5218</v>
       </c>
       <c r="D5" t="n">
-        <v>4121.65207877462</v>
+        <v>4672.20576131687</v>
       </c>
       <c r="E5" t="n">
-        <v>4121.65207877462</v>
+        <v>4672.20576131687</v>
       </c>
       <c r="F5" t="n">
-        <v>1883595</v>
+        <v>2270692</v>
       </c>
     </row>
     <row r="6">
@@ -1297,13 +1297,13 @@
         <v>17.8739</v>
       </c>
       <c r="D6" t="n">
-        <v>8048.77461706783</v>
+        <v>9258.53497942387</v>
       </c>
       <c r="E6" t="n">
-        <v>8048.77461706783</v>
+        <v>9258.53497942387</v>
       </c>
       <c r="F6" t="n">
-        <v>3678290</v>
+        <v>4499648</v>
       </c>
     </row>
     <row r="7">
@@ -1317,13 +1317,13 @@
         <v>-61.7964</v>
       </c>
       <c r="D7" t="n">
-        <v>214.319474835886</v>
+        <v>275.316872427984</v>
       </c>
       <c r="E7" t="n">
-        <v>214.319474835886</v>
+        <v>275.316872427984</v>
       </c>
       <c r="F7" t="n">
-        <v>97944</v>
+        <v>133804</v>
       </c>
     </row>
     <row r="8">
@@ -1337,13 +1337,13 @@
         <v>-63.6167</v>
       </c>
       <c r="D8" t="n">
-        <v>843185.538293217</v>
+        <v>979176.62962963</v>
       </c>
       <c r="E8" t="n">
-        <v>843185.538293217</v>
+        <v>979176.62962963</v>
       </c>
       <c r="F8" t="n">
-        <v>385335791</v>
+        <v>475879842</v>
       </c>
     </row>
     <row r="9">
@@ -1357,13 +1357,13 @@
         <v>45.0382</v>
       </c>
       <c r="D9" t="n">
-        <v>75355.1838074398</v>
+        <v>83865.3950617284</v>
       </c>
       <c r="E9" t="n">
-        <v>75355.1838074398</v>
+        <v>83865.3950617284</v>
       </c>
       <c r="F9" t="n">
-        <v>34437319</v>
+        <v>40758582</v>
       </c>
     </row>
     <row r="10">
@@ -1377,13 +1377,13 @@
         <v>149.0124</v>
       </c>
       <c r="D10" t="n">
-        <v>97.5404814004376</v>
+        <v>99.1069958847737</v>
       </c>
       <c r="E10" t="n">
-        <v>97.5404814004376</v>
+        <v>99.1069958847737</v>
       </c>
       <c r="F10" t="n">
-        <v>44576</v>
+        <v>48166</v>
       </c>
     </row>
     <row r="11">
@@ -1397,13 +1397,13 @@
         <v>151.2093</v>
       </c>
       <c r="D11" t="n">
-        <v>3595.18161925602</v>
+        <v>3709.62962962963</v>
       </c>
       <c r="E11" t="n">
-        <v>3595.18161925602</v>
+        <v>3709.62962962963</v>
       </c>
       <c r="F11" t="n">
-        <v>1642998</v>
+        <v>1802880</v>
       </c>
     </row>
     <row r="12">
@@ -1417,13 +1417,13 @@
         <v>130.8456</v>
       </c>
       <c r="D12" t="n">
-        <v>47.4857768052516</v>
+        <v>54.5946502057613</v>
       </c>
       <c r="E12" t="n">
-        <v>47.4857768052516</v>
+        <v>54.5946502057613</v>
       </c>
       <c r="F12" t="n">
-        <v>21701</v>
+        <v>26533</v>
       </c>
     </row>
     <row r="13">
@@ -1437,13 +1437,13 @@
         <v>153.0251</v>
       </c>
       <c r="D13" t="n">
-        <v>1017.69146608315</v>
+        <v>1050.6975308642</v>
       </c>
       <c r="E13" t="n">
-        <v>1017.69146608315</v>
+        <v>1050.6975308642</v>
       </c>
       <c r="F13" t="n">
-        <v>465085</v>
+        <v>510639</v>
       </c>
     </row>
     <row r="14">
@@ -1457,13 +1457,13 @@
         <v>138.6007</v>
       </c>
       <c r="D14" t="n">
-        <v>443.387308533917</v>
+        <v>460.615226337449</v>
       </c>
       <c r="E14" t="n">
-        <v>443.387308533917</v>
+        <v>460.615226337449</v>
       </c>
       <c r="F14" t="n">
-        <v>202628</v>
+        <v>223859</v>
       </c>
     </row>
     <row r="15">
@@ -1477,13 +1477,13 @@
         <v>147.3272</v>
       </c>
       <c r="D15" t="n">
-        <v>191.82056892779</v>
+        <v>194.337448559671</v>
       </c>
       <c r="E15" t="n">
-        <v>191.82056892779</v>
+        <v>194.337448559671</v>
       </c>
       <c r="F15" t="n">
-        <v>87662</v>
+        <v>94448</v>
       </c>
     </row>
     <row r="16">
@@ -1497,13 +1497,13 @@
         <v>144.9631</v>
       </c>
       <c r="D16" t="n">
-        <v>12227.5667396061</v>
+        <v>12722.9526748971</v>
       </c>
       <c r="E16" t="n">
-        <v>12227.5667396061</v>
+        <v>12722.9526748971</v>
       </c>
       <c r="F16" t="n">
-        <v>5587998</v>
+        <v>6183355</v>
       </c>
     </row>
     <row r="17">
@@ -1517,13 +1517,13 @@
         <v>115.8605</v>
       </c>
       <c r="D17" t="n">
-        <v>630.835886214442</v>
+        <v>653.298353909465</v>
       </c>
       <c r="E17" t="n">
-        <v>630.835886214442</v>
+        <v>653.298353909465</v>
       </c>
       <c r="F17" t="n">
-        <v>288292</v>
+        <v>317503</v>
       </c>
     </row>
     <row r="18">
@@ -1537,13 +1537,13 @@
         <v>14.5501</v>
       </c>
       <c r="D18" t="n">
-        <v>163371.820568928</v>
+        <v>191000.156378601</v>
       </c>
       <c r="E18" t="n">
-        <v>163371.820568928</v>
+        <v>191000.156378601</v>
       </c>
       <c r="F18" t="n">
-        <v>74660922</v>
+        <v>92826076</v>
       </c>
     </row>
     <row r="19">
@@ -1557,13 +1557,13 @@
         <v>47.5769</v>
       </c>
       <c r="D19" t="n">
-        <v>88223.4026258206</v>
+        <v>102269.316872428</v>
       </c>
       <c r="E19" t="n">
-        <v>88223.4026258206</v>
+        <v>102269.316872428</v>
       </c>
       <c r="F19" t="n">
-        <v>40318095</v>
+        <v>49702888</v>
       </c>
     </row>
     <row r="20">
@@ -1577,13 +1577,13 @@
         <v>-78.035889</v>
       </c>
       <c r="D20" t="n">
-        <v>3799.92560175055</v>
+        <v>4212.72222222222</v>
       </c>
       <c r="E20" t="n">
-        <v>3799.92560175055</v>
+        <v>4212.72222222222</v>
       </c>
       <c r="F20" t="n">
-        <v>1736566</v>
+        <v>2047383</v>
       </c>
     </row>
     <row r="21">
@@ -1597,13 +1597,13 @@
         <v>50.55</v>
       </c>
       <c r="D21" t="n">
-        <v>58403.7352297593</v>
+        <v>66118.0452674897</v>
       </c>
       <c r="E21" t="n">
-        <v>58403.7352297593</v>
+        <v>66118.0452674897</v>
       </c>
       <c r="F21" t="n">
-        <v>26690507</v>
+        <v>32133370</v>
       </c>
     </row>
     <row r="22">
@@ -1617,13 +1617,13 @@
         <v>90.3563</v>
       </c>
       <c r="D22" t="n">
-        <v>290775.076586433</v>
+        <v>319244.611111111</v>
       </c>
       <c r="E22" t="n">
-        <v>290775.076586433</v>
+        <v>319244.611111111</v>
       </c>
       <c r="F22" t="n">
-        <v>132884210</v>
+        <v>155152881</v>
       </c>
     </row>
     <row r="23">
@@ -1637,13 +1637,13 @@
         <v>-59.5432</v>
       </c>
       <c r="D23" t="n">
-        <v>720.754923413567</v>
+        <v>911.008230452675</v>
       </c>
       <c r="E23" t="n">
-        <v>720.754923413567</v>
+        <v>911.008230452675</v>
       </c>
       <c r="F23" t="n">
-        <v>329385</v>
+        <v>442750</v>
       </c>
     </row>
     <row r="24">
@@ -1657,13 +1657,13 @@
         <v>27.9534</v>
       </c>
       <c r="D24" t="n">
-        <v>113141.518599562</v>
+        <v>128245.934156379</v>
       </c>
       <c r="E24" t="n">
-        <v>113141.518599562</v>
+        <v>128245.934156379</v>
       </c>
       <c r="F24" t="n">
-        <v>51705674</v>
+        <v>62327524</v>
       </c>
     </row>
     <row r="25">
@@ -1677,13 +1677,13 @@
         <v>4.469936</v>
       </c>
       <c r="D25" t="n">
-        <v>309297.024070022</v>
+        <v>351003.121399177</v>
       </c>
       <c r="E25" t="n">
-        <v>309297.024070022</v>
+        <v>351003.121399177</v>
       </c>
       <c r="F25" t="n">
-        <v>141348740</v>
+        <v>170587517</v>
       </c>
     </row>
     <row r="26">
@@ -1697,13 +1697,13 @@
         <v>-88.4976</v>
       </c>
       <c r="D26" t="n">
-        <v>4221.64332603939</v>
+        <v>4726.60082304527</v>
       </c>
       <c r="E26" t="n">
-        <v>4221.64332603939</v>
+        <v>4726.60082304527</v>
       </c>
       <c r="F26" t="n">
-        <v>1929291</v>
+        <v>2297128</v>
       </c>
     </row>
     <row r="27">
@@ -1717,13 +1717,13 @@
         <v>2.3158</v>
       </c>
       <c r="D27" t="n">
-        <v>2346.36323851203</v>
+        <v>2677.22222222222</v>
       </c>
       <c r="E27" t="n">
-        <v>2346.36323851203</v>
+        <v>2677.22222222222</v>
       </c>
       <c r="F27" t="n">
-        <v>1072288</v>
+        <v>1301130</v>
       </c>
     </row>
     <row r="28">
@@ -1737,13 +1737,13 @@
         <v>90.4336</v>
       </c>
       <c r="D28" t="n">
-        <v>328.652078774617</v>
+        <v>379.417695473251</v>
       </c>
       <c r="E28" t="n">
-        <v>328.652078774617</v>
+        <v>379.417695473251</v>
       </c>
       <c r="F28" t="n">
-        <v>150194</v>
+        <v>184397</v>
       </c>
     </row>
     <row r="29">
@@ -1757,13 +1757,13 @@
         <v>-63.5887</v>
       </c>
       <c r="D29" t="n">
-        <v>107934.903719912</v>
+        <v>120359.33127572</v>
       </c>
       <c r="E29" t="n">
-        <v>107934.903719912</v>
+        <v>120359.33127572</v>
       </c>
       <c r="F29" t="n">
-        <v>49326251</v>
+        <v>58494635</v>
       </c>
     </row>
     <row r="30">
@@ -1777,13 +1777,13 @@
         <v>17.6791</v>
       </c>
       <c r="D30" t="n">
-        <v>52152.7921225383</v>
+        <v>60964.4650205761</v>
       </c>
       <c r="E30" t="n">
-        <v>52152.7921225383</v>
+        <v>60964.4650205761</v>
       </c>
       <c r="F30" t="n">
-        <v>23833826</v>
+        <v>29628730</v>
       </c>
     </row>
     <row r="31">
@@ -1797,13 +1797,13 @@
         <v>24.6849</v>
       </c>
       <c r="D31" t="n">
-        <v>9273.36761487965</v>
+        <v>11605.5102880658</v>
       </c>
       <c r="E31" t="n">
-        <v>9273.36761487965</v>
+        <v>11605.5102880658</v>
       </c>
       <c r="F31" t="n">
-        <v>4237929</v>
+        <v>5640278</v>
       </c>
     </row>
     <row r="32">
@@ -1817,13 +1817,13 @@
         <v>-51.9253</v>
       </c>
       <c r="D32" t="n">
-        <v>4566029.63238512</v>
+        <v>5192786.95473251</v>
       </c>
       <c r="E32" t="n">
-        <v>4566029.63238512</v>
+        <v>5192786.95473251</v>
       </c>
       <c r="F32" t="n">
-        <v>2086675542</v>
+        <v>2523694460</v>
       </c>
     </row>
     <row r="33">
@@ -1837,13 +1837,13 @@
         <v>114.7277</v>
       </c>
       <c r="D33" t="n">
-        <v>137.18818380744</v>
+        <v>142.641975308642</v>
       </c>
       <c r="E33" t="n">
-        <v>137.18818380744</v>
+        <v>142.641975308642</v>
       </c>
       <c r="F33" t="n">
-        <v>62695</v>
+        <v>69324</v>
       </c>
     </row>
     <row r="34">
@@ -1857,13 +1857,13 @@
         <v>25.4858</v>
       </c>
       <c r="D34" t="n">
-        <v>90484.7264770241</v>
+        <v>109447.117283951</v>
       </c>
       <c r="E34" t="n">
-        <v>90484.7264770241</v>
+        <v>109447.117283951</v>
       </c>
       <c r="F34" t="n">
-        <v>41351520</v>
+        <v>53191299</v>
       </c>
     </row>
     <row r="35">
@@ -1877,13 +1877,13 @@
         <v>-1.5616</v>
       </c>
       <c r="D35" t="n">
-        <v>3840.14442013129</v>
+        <v>4407.329218107</v>
       </c>
       <c r="E35" t="n">
-        <v>3840.14442013129</v>
+        <v>4407.329218107</v>
       </c>
       <c r="F35" t="n">
-        <v>1754946</v>
+        <v>2141962</v>
       </c>
     </row>
     <row r="36">
@@ -1897,13 +1897,13 @@
         <v>95.956</v>
       </c>
       <c r="D36" t="n">
-        <v>49072.5032822757</v>
+        <v>54672.6028806584</v>
       </c>
       <c r="E36" t="n">
-        <v>49072.5032822757</v>
+        <v>54672.6028806584</v>
       </c>
       <c r="F36" t="n">
-        <v>22426134</v>
+        <v>26570885</v>
       </c>
     </row>
     <row r="37">
@@ -1917,13 +1917,13 @@
         <v>29.9189</v>
       </c>
       <c r="D37" t="n">
-        <v>736.039387308534</v>
+        <v>938.259259259259</v>
       </c>
       <c r="E37" t="n">
-        <v>736.039387308534</v>
+        <v>938.259259259259</v>
       </c>
       <c r="F37" t="n">
-        <v>336370</v>
+        <v>455994</v>
       </c>
     </row>
     <row r="38">
@@ -1937,13 +1937,13 @@
         <v>-23.0418</v>
       </c>
       <c r="D38" t="n">
-        <v>6476.19474835886</v>
+        <v>7620.3621399177</v>
       </c>
       <c r="E38" t="n">
-        <v>6476.19474835886</v>
+        <v>7620.3621399177</v>
       </c>
       <c r="F38" t="n">
-        <v>2959621</v>
+        <v>3703496</v>
       </c>
     </row>
     <row r="39">
@@ -1957,13 +1957,13 @@
         <v>104.9167</v>
       </c>
       <c r="D39" t="n">
-        <v>525.35010940919</v>
+        <v>1527.30864197531</v>
       </c>
       <c r="E39" t="n">
-        <v>525.35010940919</v>
+        <v>1527.30864197531</v>
       </c>
       <c r="F39" t="n">
-        <v>240085</v>
+        <v>742272</v>
       </c>
     </row>
     <row r="40">
@@ -1977,13 +1977,13 @@
         <v>11.5021</v>
       </c>
       <c r="D40" t="n">
-        <v>18843.9212253829</v>
+        <v>22063.3374485597</v>
       </c>
       <c r="E40" t="n">
-        <v>18843.9212253829</v>
+        <v>22063.3374485597</v>
       </c>
       <c r="F40" t="n">
-        <v>8611672</v>
+        <v>10722782</v>
       </c>
     </row>
     <row r="41">
@@ -1997,13 +1997,13 @@
         <v>-116.5765</v>
       </c>
       <c r="D41" t="n">
-        <v>46401.8840262582</v>
+        <v>55763.5802469136</v>
       </c>
       <c r="E41" t="n">
-        <v>46401.8840262582</v>
+        <v>55763.5802469136</v>
       </c>
       <c r="F41" t="n">
-        <v>21205661</v>
+        <v>27101100</v>
       </c>
     </row>
     <row r="42">
@@ -2017,13 +2017,13 @@
         <v>-127.6476</v>
       </c>
       <c r="D42" t="n">
-        <v>26686.9146608315</v>
+        <v>33054.487654321</v>
       </c>
       <c r="E42" t="n">
-        <v>26686.9146608315</v>
+        <v>33054.487654321</v>
       </c>
       <c r="F42" t="n">
-        <v>12195920</v>
+        <v>16064481</v>
       </c>
     </row>
     <row r="43">
@@ -2037,10 +2037,10 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0700218818380744</v>
+        <v>0.065843621399177</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0700218818380744</v>
+        <v>0.065843621399177</v>
       </c>
       <c r="F43" t="n">
         <v>32</v>
@@ -2057,13 +2057,13 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>11.4113785557987</v>
+        <v>11.5061728395062</v>
       </c>
       <c r="E44" t="n">
-        <v>11.4113785557987</v>
+        <v>11.5061728395062</v>
       </c>
       <c r="F44" t="n">
-        <v>5215</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="45">
@@ -2077,13 +2077,13 @@
         <v>-98.8139</v>
       </c>
       <c r="D45" t="n">
-        <v>10314.4245076586</v>
+        <v>12176.1646090535</v>
       </c>
       <c r="E45" t="n">
-        <v>10314.4245076586</v>
+        <v>12176.1646090535</v>
       </c>
       <c r="F45" t="n">
-        <v>4713692</v>
+        <v>5917616</v>
       </c>
     </row>
     <row r="46">
@@ -2097,13 +2097,13 @@
         <v>-66.4619</v>
       </c>
       <c r="D46" t="n">
-        <v>477.98249452954</v>
+        <v>567.590534979424</v>
       </c>
       <c r="E46" t="n">
-        <v>477.98249452954</v>
+        <v>567.590534979424</v>
       </c>
       <c r="F46" t="n">
-        <v>218438</v>
+        <v>275849</v>
       </c>
     </row>
     <row r="47">
@@ -2117,13 +2117,13 @@
         <v>-57.6604</v>
       </c>
       <c r="D47" t="n">
-        <v>358</v>
+        <v>404.092592592593</v>
       </c>
       <c r="E47" t="n">
-        <v>358</v>
+        <v>404.092592592593</v>
       </c>
       <c r="F47" t="n">
-        <v>163606</v>
+        <v>196389</v>
       </c>
     </row>
     <row r="48">
@@ -2137,13 +2137,13 @@
         <v>-124.8457</v>
       </c>
       <c r="D48" t="n">
-        <v>14.6673960612691</v>
+        <v>19.2901234567901</v>
       </c>
       <c r="E48" t="n">
-        <v>14.6673960612691</v>
+        <v>19.2901234567901</v>
       </c>
       <c r="F48" t="n">
-        <v>6703</v>
+        <v>9375</v>
       </c>
     </row>
     <row r="49">
@@ -2157,13 +2157,13 @@
         <v>-63.7443</v>
       </c>
       <c r="D49" t="n">
-        <v>1044.5295404814</v>
+        <v>1192.22633744856</v>
       </c>
       <c r="E49" t="n">
-        <v>1044.5295404814</v>
+        <v>1192.22633744856</v>
       </c>
       <c r="F49" t="n">
-        <v>477350</v>
+        <v>579422</v>
       </c>
     </row>
     <row r="50">
@@ -2177,13 +2177,13 @@
         <v>-83.1076</v>
       </c>
       <c r="D50" t="n">
-        <v>104.111597374179</v>
+        <v>130.810699588477</v>
       </c>
       <c r="E50" t="n">
-        <v>104.111597374179</v>
+        <v>130.810699588477</v>
       </c>
       <c r="F50" t="n">
-        <v>47579</v>
+        <v>63574</v>
       </c>
     </row>
     <row r="51">
@@ -2197,13 +2197,13 @@
         <v>-85.3232</v>
       </c>
       <c r="D51" t="n">
-        <v>109560.89059081</v>
+        <v>132339.557613169</v>
       </c>
       <c r="E51" t="n">
-        <v>109560.89059081</v>
+        <v>132339.557613169</v>
       </c>
       <c r="F51" t="n">
-        <v>50069327</v>
+        <v>64317025</v>
       </c>
     </row>
     <row r="52">
@@ -2217,13 +2217,13 @@
         <v>-63.4168</v>
       </c>
       <c r="D52" t="n">
-        <v>60.45295404814</v>
+        <v>67.7921810699588</v>
       </c>
       <c r="E52" t="n">
-        <v>60.45295404814</v>
+        <v>67.7921810699588</v>
       </c>
       <c r="F52" t="n">
-        <v>27627</v>
+        <v>32947</v>
       </c>
     </row>
     <row r="53">
@@ -2237,13 +2237,13 @@
         <v>-73.5491</v>
       </c>
       <c r="D53" t="n">
-        <v>114806.566739606</v>
+        <v>129174.664609053</v>
       </c>
       <c r="E53" t="n">
-        <v>114806.566739606</v>
+        <v>129174.664609053</v>
       </c>
       <c r="F53" t="n">
-        <v>52466601</v>
+        <v>62778887</v>
       </c>
     </row>
     <row r="54">
@@ -2253,13 +2253,13 @@
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54" t="n">
-        <v>4.26695842450766</v>
+        <v>4.7880658436214</v>
       </c>
       <c r="E54" t="n">
-        <v>4.26695842450766</v>
+        <v>4.7880658436214</v>
       </c>
       <c r="F54" t="n">
-        <v>1950</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="55">
@@ -2273,13 +2273,13 @@
         <v>-106.4509</v>
       </c>
       <c r="D55" t="n">
-        <v>8567.09190371991</v>
+        <v>10596.3456790123</v>
       </c>
       <c r="E55" t="n">
-        <v>8567.09190371991</v>
+        <v>10596.3456790123</v>
       </c>
       <c r="F55" t="n">
-        <v>3915161</v>
+        <v>5149824</v>
       </c>
     </row>
     <row r="56">
@@ -2293,13 +2293,13 @@
         <v>-135</v>
       </c>
       <c r="D56" t="n">
-        <v>29.4201312910284</v>
+        <v>32.5761316872428</v>
       </c>
       <c r="E56" t="n">
-        <v>29.4201312910284</v>
+        <v>32.5761316872428</v>
       </c>
       <c r="F56" t="n">
-        <v>13445</v>
+        <v>15832</v>
       </c>
     </row>
     <row r="57">
@@ -2313,13 +2313,13 @@
         <v>20.9394</v>
       </c>
       <c r="D57" t="n">
-        <v>3344.09409190372</v>
+        <v>3539.59259259259</v>
       </c>
       <c r="E57" t="n">
-        <v>3344.09409190372</v>
+        <v>3539.59259259259</v>
       </c>
       <c r="F57" t="n">
-        <v>1528251</v>
+        <v>1720242</v>
       </c>
     </row>
     <row r="58">
@@ -2333,13 +2333,13 @@
         <v>18.7322</v>
       </c>
       <c r="D58" t="n">
-        <v>1539.70021881838</v>
+        <v>1737.2962962963</v>
       </c>
       <c r="E58" t="n">
-        <v>1539.70021881838</v>
+        <v>1737.2962962963</v>
       </c>
       <c r="F58" t="n">
-        <v>703643</v>
+        <v>844326</v>
       </c>
     </row>
     <row r="59">
@@ -2353,13 +2353,13 @@
         <v>-71.543</v>
       </c>
       <c r="D59" t="n">
-        <v>408387.516411379</v>
+        <v>457750.495884774</v>
       </c>
       <c r="E59" t="n">
-        <v>408387.516411379</v>
+        <v>457750.495884774</v>
       </c>
       <c r="F59" t="n">
-        <v>186633095</v>
+        <v>222466741</v>
       </c>
     </row>
     <row r="60">
@@ -2373,13 +2373,13 @@
         <v>117.2264</v>
       </c>
       <c r="D60" t="n">
-        <v>961.597374179431</v>
+        <v>963.641975308642</v>
       </c>
       <c r="E60" t="n">
-        <v>961.597374179431</v>
+        <v>963.641975308642</v>
       </c>
       <c r="F60" t="n">
-        <v>439450</v>
+        <v>468330</v>
       </c>
     </row>
     <row r="61">
@@ -2393,13 +2393,13 @@
         <v>116.4142</v>
       </c>
       <c r="D61" t="n">
-        <v>815.886214442013</v>
+        <v>830.27366255144</v>
       </c>
       <c r="E61" t="n">
-        <v>815.886214442013</v>
+        <v>830.27366255144</v>
       </c>
       <c r="F61" t="n">
-        <v>372860</v>
+        <v>403513</v>
       </c>
     </row>
     <row r="62">
@@ -2413,13 +2413,13 @@
         <v>107.874</v>
       </c>
       <c r="D62" t="n">
-        <v>568.958424507659</v>
+        <v>570.61316872428</v>
       </c>
       <c r="E62" t="n">
-        <v>568.958424507659</v>
+        <v>570.61316872428</v>
       </c>
       <c r="F62" t="n">
-        <v>260014</v>
+        <v>277318</v>
       </c>
     </row>
     <row r="63">
@@ -2433,13 +2433,13 @@
         <v>117.9874</v>
       </c>
       <c r="D63" t="n">
-        <v>413.216630196937</v>
+        <v>424.08024691358</v>
       </c>
       <c r="E63" t="n">
-        <v>413.216630196937</v>
+        <v>424.08024691358</v>
       </c>
       <c r="F63" t="n">
-        <v>188840</v>
+        <v>206103</v>
       </c>
     </row>
     <row r="64">
@@ -2453,13 +2453,13 @@
         <v>104.2861</v>
       </c>
       <c r="D64" t="n">
-        <v>157.827133479212</v>
+        <v>159.925925925926</v>
       </c>
       <c r="E64" t="n">
-        <v>157.827133479212</v>
+        <v>159.925925925926</v>
       </c>
       <c r="F64" t="n">
-        <v>72127</v>
+        <v>77724</v>
       </c>
     </row>
     <row r="65">
@@ -2473,13 +2473,13 @@
         <v>113.4244</v>
       </c>
       <c r="D65" t="n">
-        <v>1765.97374179431</v>
+        <v>1801.78395061728</v>
       </c>
       <c r="E65" t="n">
-        <v>1765.97374179431</v>
+        <v>1801.78395061728</v>
       </c>
       <c r="F65" t="n">
-        <v>807050</v>
+        <v>875667</v>
       </c>
     </row>
     <row r="66">
@@ -2493,13 +2493,13 @@
         <v>108.7881</v>
       </c>
       <c r="D66" t="n">
-        <v>251.63238512035</v>
+        <v>252.940329218107</v>
       </c>
       <c r="E66" t="n">
-        <v>251.63238512035</v>
+        <v>252.940329218107</v>
       </c>
       <c r="F66" t="n">
-        <v>114996</v>
+        <v>122929</v>
       </c>
     </row>
     <row r="67">
@@ -2513,13 +2513,13 @@
         <v>106.8748</v>
       </c>
       <c r="D67" t="n">
-        <v>141.978118161926</v>
+        <v>142.277777777778</v>
       </c>
       <c r="E67" t="n">
-        <v>141.978118161926</v>
+        <v>142.277777777778</v>
       </c>
       <c r="F67" t="n">
-        <v>64884</v>
+        <v>69147</v>
       </c>
     </row>
     <row r="68">
@@ -2533,13 +2533,13 @@
         <v>109.7453</v>
       </c>
       <c r="D68" t="n">
-        <v>165.512035010941</v>
+        <v>166.841563786008</v>
       </c>
       <c r="E68" t="n">
-        <v>165.512035010941</v>
+        <v>166.841563786008</v>
       </c>
       <c r="F68" t="n">
-        <v>75639</v>
+        <v>81085</v>
       </c>
     </row>
     <row r="69">
@@ -2553,13 +2553,13 @@
         <v>116.1306</v>
       </c>
       <c r="D69" t="n">
-        <v>547.037199124726</v>
+        <v>592.981481481482</v>
       </c>
       <c r="E69" t="n">
-        <v>547.037199124726</v>
+        <v>592.981481481482</v>
       </c>
       <c r="F69" t="n">
-        <v>249996</v>
+        <v>288189</v>
       </c>
     </row>
     <row r="70">
@@ -2573,13 +2573,13 @@
         <v>127.7615</v>
       </c>
       <c r="D70" t="n">
-        <v>980.428884026258</v>
+        <v>1018.00617283951</v>
       </c>
       <c r="E70" t="n">
-        <v>980.428884026258</v>
+        <v>1018.00617283951</v>
       </c>
       <c r="F70" t="n">
-        <v>448056</v>
+        <v>494751</v>
       </c>
     </row>
     <row r="71">
@@ -2593,13 +2593,13 @@
         <v>114.9042</v>
       </c>
       <c r="D71" t="n">
-        <v>1248.08315098468</v>
+        <v>1251.91563786008</v>
       </c>
       <c r="E71" t="n">
-        <v>1248.08315098468</v>
+        <v>1251.91563786008</v>
       </c>
       <c r="F71" t="n">
-        <v>570374</v>
+        <v>608431</v>
       </c>
     </row>
     <row r="72">
@@ -2613,13 +2613,13 @@
         <v>114.2</v>
       </c>
       <c r="D72" t="n">
-        <v>4857.87527352298</v>
+        <v>5271.66872427984</v>
       </c>
       <c r="E72" t="n">
-        <v>4857.87527352298</v>
+        <v>5271.66872427984</v>
       </c>
       <c r="F72" t="n">
-        <v>2220049</v>
+        <v>2562031</v>
       </c>
     </row>
     <row r="73">
@@ -2633,13 +2633,13 @@
         <v>112.2707</v>
       </c>
       <c r="D73" t="n">
-        <v>65214.4442013129</v>
+        <v>65390.0864197531</v>
       </c>
       <c r="E73" t="n">
-        <v>65214.4442013129</v>
+        <v>65390.0864197531</v>
       </c>
       <c r="F73" t="n">
-        <v>29803001</v>
+        <v>31779582</v>
       </c>
     </row>
     <row r="74">
@@ -2653,13 +2653,13 @@
         <v>111.7088</v>
       </c>
       <c r="D74" t="n">
-        <v>994.667396061269</v>
+        <v>997.69341563786</v>
       </c>
       <c r="E74" t="n">
-        <v>994.667396061269</v>
+        <v>997.69341563786</v>
       </c>
       <c r="F74" t="n">
-        <v>454563</v>
+        <v>484879</v>
       </c>
     </row>
     <row r="75">
@@ -2673,13 +2673,13 @@
         <v>113.9448</v>
       </c>
       <c r="D75" t="n">
-        <v>254.89715536105</v>
+        <v>262.469135802469</v>
       </c>
       <c r="E75" t="n">
-        <v>254.89715536105</v>
+        <v>262.469135802469</v>
       </c>
       <c r="F75" t="n">
-        <v>116488</v>
+        <v>127560</v>
       </c>
     </row>
     <row r="76">
@@ -2693,13 +2693,13 @@
         <v>119.455</v>
       </c>
       <c r="D76" t="n">
-        <v>648.553610503282</v>
+        <v>652.810699588477</v>
       </c>
       <c r="E76" t="n">
-        <v>648.553610503282</v>
+        <v>652.810699588477</v>
       </c>
       <c r="F76" t="n">
-        <v>296389</v>
+        <v>317266</v>
       </c>
     </row>
     <row r="77">
@@ -2713,13 +2713,13 @@
         <v>115.7221</v>
       </c>
       <c r="D77" t="n">
-        <v>906.945295404814</v>
+        <v>908.738683127572</v>
       </c>
       <c r="E77" t="n">
-        <v>906.945295404814</v>
+        <v>908.738683127572</v>
       </c>
       <c r="F77" t="n">
-        <v>414474</v>
+        <v>441647</v>
       </c>
     </row>
     <row r="78">
@@ -2733,13 +2733,13 @@
         <v>126.1923</v>
       </c>
       <c r="D78" t="n">
-        <v>220.667396061269</v>
+        <v>241.691358024691</v>
       </c>
       <c r="E78" t="n">
-        <v>220.667396061269</v>
+        <v>241.691358024691</v>
       </c>
       <c r="F78" t="n">
-        <v>100845</v>
+        <v>117462</v>
       </c>
     </row>
     <row r="79">
@@ -2753,13 +2753,13 @@
         <v>122.6085</v>
       </c>
       <c r="D79" t="n">
-        <v>248.890590809628</v>
+        <v>258.578189300412</v>
       </c>
       <c r="E79" t="n">
-        <v>248.890590809628</v>
+        <v>258.578189300412</v>
       </c>
       <c r="F79" t="n">
-        <v>113743</v>
+        <v>125669</v>
       </c>
     </row>
     <row r="80">
@@ -2773,13 +2773,13 @@
         <v>113.55</v>
       </c>
       <c r="D80" t="n">
-        <v>41.0853391684902</v>
+        <v>41.5699588477366</v>
       </c>
       <c r="E80" t="n">
-        <v>41.0853391684902</v>
+        <v>41.5699588477366</v>
       </c>
       <c r="F80" t="n">
-        <v>18776</v>
+        <v>20203</v>
       </c>
     </row>
     <row r="81">
@@ -2793,13 +2793,13 @@
         <v>106.1655</v>
       </c>
       <c r="D81" t="n">
-        <v>72.4442013129103</v>
+        <v>72.6255144032922</v>
       </c>
       <c r="E81" t="n">
-        <v>72.4442013129103</v>
+        <v>72.6255144032922</v>
       </c>
       <c r="F81" t="n">
-        <v>33107</v>
+        <v>35296</v>
       </c>
     </row>
     <row r="82">
@@ -2813,13 +2813,13 @@
         <v>95.9956</v>
       </c>
       <c r="D82" t="n">
-        <v>17.6301969365427</v>
+        <v>17.6522633744856</v>
       </c>
       <c r="E82" t="n">
-        <v>17.6301969365427</v>
+        <v>17.6522633744856</v>
       </c>
       <c r="F82" t="n">
-        <v>8057</v>
+        <v>8579</v>
       </c>
     </row>
     <row r="83">
@@ -2833,13 +2833,13 @@
         <v>108.8701</v>
       </c>
       <c r="D83" t="n">
-        <v>391.223194748359</v>
+        <v>403.384773662551</v>
       </c>
       <c r="E83" t="n">
-        <v>391.223194748359</v>
+        <v>403.384773662551</v>
       </c>
       <c r="F83" t="n">
-        <v>178789</v>
+        <v>196045</v>
       </c>
     </row>
     <row r="84">
@@ -2853,13 +2853,13 @@
         <v>118.1498</v>
       </c>
       <c r="D84" t="n">
-        <v>791.868708971554</v>
+        <v>797.074074074074</v>
       </c>
       <c r="E84" t="n">
-        <v>791.868708971554</v>
+        <v>797.074074074074</v>
       </c>
       <c r="F84" t="n">
-        <v>361884</v>
+        <v>387378</v>
       </c>
     </row>
     <row r="85">
@@ -2873,13 +2873,13 @@
         <v>121.4491</v>
       </c>
       <c r="D85" t="n">
-        <v>1032.40700218818</v>
+        <v>1090.68518518519</v>
       </c>
       <c r="E85" t="n">
-        <v>1032.40700218818</v>
+        <v>1090.68518518519</v>
       </c>
       <c r="F85" t="n">
-        <v>471810</v>
+        <v>530073</v>
       </c>
     </row>
     <row r="86">
@@ -2893,13 +2893,13 @@
         <v>112.2922</v>
       </c>
       <c r="D86" t="n">
-        <v>197.409190371991</v>
+        <v>200.584362139918</v>
       </c>
       <c r="E86" t="n">
-        <v>197.409190371991</v>
+        <v>200.584362139918</v>
       </c>
       <c r="F86" t="n">
-        <v>90216</v>
+        <v>97484</v>
       </c>
     </row>
     <row r="87">
@@ -2913,13 +2913,13 @@
         <v>102.7103</v>
       </c>
       <c r="D87" t="n">
-        <v>685.122538293217</v>
+        <v>703.341563786008</v>
       </c>
       <c r="E87" t="n">
-        <v>685.122538293217</v>
+        <v>703.341563786008</v>
       </c>
       <c r="F87" t="n">
-        <v>313101</v>
+        <v>341824</v>
       </c>
     </row>
     <row r="88">
@@ -2933,13 +2933,13 @@
         <v>117.323</v>
       </c>
       <c r="D88" t="n">
-        <v>241.520787746171</v>
+        <v>250.166666666667</v>
       </c>
       <c r="E88" t="n">
-        <v>241.520787746171</v>
+        <v>250.166666666667</v>
       </c>
       <c r="F88" t="n">
-        <v>110375</v>
+        <v>121581</v>
       </c>
     </row>
     <row r="89">
@@ -2953,13 +2953,13 @@
         <v>88.0924</v>
       </c>
       <c r="D89" t="n">
-        <v>0.982494529540481</v>
+        <v>0.983539094650206</v>
       </c>
       <c r="E89" t="n">
-        <v>0.982494529540481</v>
+        <v>0.983539094650206</v>
       </c>
       <c r="F89" t="n">
-        <v>449</v>
+        <v>478</v>
       </c>
     </row>
     <row r="90">
@@ -2969,13 +2969,13 @@
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90" t="n">
-        <v>2.30853391684902</v>
+        <v>0.01440329218107</v>
       </c>
       <c r="E90" t="n">
-        <v>2.30853391684902</v>
+        <v>0.01440329218107</v>
       </c>
       <c r="F90" t="n">
-        <v>1055</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
@@ -2989,13 +2989,13 @@
         <v>85.2401</v>
       </c>
       <c r="D91" t="n">
-        <v>585.763676148797</v>
+        <v>609.288065843621</v>
       </c>
       <c r="E91" t="n">
-        <v>585.763676148797</v>
+        <v>609.288065843621</v>
       </c>
       <c r="F91" t="n">
-        <v>267694</v>
+        <v>296114</v>
       </c>
     </row>
     <row r="92">
@@ -3009,13 +3009,13 @@
         <v>101.487</v>
       </c>
       <c r="D92" t="n">
-        <v>203.08533916849</v>
+        <v>211.621399176955</v>
       </c>
       <c r="E92" t="n">
-        <v>203.08533916849</v>
+        <v>211.621399176955</v>
       </c>
       <c r="F92" t="n">
-        <v>92810</v>
+        <v>102848</v>
       </c>
     </row>
     <row r="93">
@@ -3029,13 +3029,13 @@
         <v>120.0934</v>
       </c>
       <c r="D93" t="n">
-        <v>1247.99124726477</v>
+        <v>1253.80658436214</v>
       </c>
       <c r="E93" t="n">
-        <v>1247.99124726477</v>
+        <v>1253.80658436214</v>
       </c>
       <c r="F93" t="n">
-        <v>570332</v>
+        <v>609350</v>
       </c>
     </row>
     <row r="94">
@@ -3049,13 +3049,13 @@
         <v>-74.2973</v>
       </c>
       <c r="D94" t="n">
-        <v>882083.70678337</v>
+        <v>1006621.98559671</v>
       </c>
       <c r="E94" t="n">
-        <v>882083.70678337</v>
+        <v>1006621.98559671</v>
       </c>
       <c r="F94" t="n">
-        <v>403112254</v>
+        <v>489218285</v>
       </c>
     </row>
     <row r="95">
@@ -3069,13 +3069,13 @@
         <v>43.3333</v>
       </c>
       <c r="D95" t="n">
-        <v>956.415754923414</v>
+        <v>1129.00823045267</v>
       </c>
       <c r="E95" t="n">
-        <v>956.415754923414</v>
+        <v>1129.00823045267</v>
       </c>
       <c r="F95" t="n">
-        <v>437082</v>
+        <v>548698</v>
       </c>
     </row>
     <row r="96">
@@ -3089,13 +3089,13 @@
         <v>15.8277</v>
       </c>
       <c r="D96" t="n">
-        <v>4101.57549234136</v>
+        <v>4514.46913580247</v>
       </c>
       <c r="E96" t="n">
-        <v>4101.57549234136</v>
+        <v>4514.46913580247</v>
       </c>
       <c r="F96" t="n">
-        <v>1874420</v>
+        <v>2194032</v>
       </c>
     </row>
     <row r="97">
@@ -3109,13 +3109,13 @@
         <v>21.7587</v>
       </c>
       <c r="D97" t="n">
-        <v>10994.124726477</v>
+        <v>12138.7839506173</v>
       </c>
       <c r="E97" t="n">
-        <v>10994.124726477</v>
+        <v>12138.7839506173</v>
       </c>
       <c r="F97" t="n">
-        <v>5024315</v>
+        <v>5899449</v>
       </c>
     </row>
     <row r="98">
@@ -3129,13 +3129,13 @@
         <v>-83.7534</v>
       </c>
       <c r="D98" t="n">
-        <v>81479.9978118162</v>
+        <v>92461.646090535</v>
       </c>
       <c r="E98" t="n">
-        <v>81479.9978118162</v>
+        <v>92461.646090535</v>
       </c>
       <c r="F98" t="n">
-        <v>37236359</v>
+        <v>44936360</v>
       </c>
     </row>
     <row r="99">
@@ -3149,13 +3149,13 @@
         <v>-5.5471</v>
       </c>
       <c r="D99" t="n">
-        <v>16484.5601750547</v>
+        <v>18264.2407407407</v>
       </c>
       <c r="E99" t="n">
-        <v>16484.5601750547</v>
+        <v>18264.2407407407</v>
       </c>
       <c r="F99" t="n">
-        <v>7533444</v>
+        <v>8876421</v>
       </c>
     </row>
     <row r="100">
@@ -3169,13 +3169,13 @@
         <v>15.2</v>
       </c>
       <c r="D100" t="n">
-        <v>82811.5142231948</v>
+        <v>98134.1419753086</v>
       </c>
       <c r="E100" t="n">
-        <v>82811.5142231948</v>
+        <v>98134.1419753086</v>
       </c>
       <c r="F100" t="n">
-        <v>37844862</v>
+        <v>47693193</v>
       </c>
     </row>
     <row r="101">
@@ -3189,13 +3189,13 @@
         <v>-77.781167</v>
       </c>
       <c r="D101" t="n">
-        <v>14677.47702407</v>
+        <v>20621.7386831276</v>
       </c>
       <c r="E101" t="n">
-        <v>14677.47702407</v>
+        <v>20621.7386831276</v>
       </c>
       <c r="F101" t="n">
-        <v>6707607</v>
+        <v>10022165</v>
       </c>
     </row>
     <row r="102">
@@ -3209,13 +3209,13 @@
         <v>33.4299</v>
       </c>
       <c r="D102" t="n">
-        <v>11359.9649890591</v>
+        <v>14730.8127572016</v>
       </c>
       <c r="E102" t="n">
-        <v>11359.9649890591</v>
+        <v>14730.8127572016</v>
       </c>
       <c r="F102" t="n">
-        <v>5191504</v>
+        <v>7159175</v>
       </c>
     </row>
     <row r="103">
@@ -3229,13 +3229,13 @@
         <v>15.473</v>
       </c>
       <c r="D103" t="n">
-        <v>387383.216630197</v>
+        <v>462118.148148148</v>
       </c>
       <c r="E103" t="n">
-        <v>387383.216630197</v>
+        <v>462118.148148148</v>
       </c>
       <c r="F103" t="n">
-        <v>177034130</v>
+        <v>224589420</v>
       </c>
     </row>
     <row r="104">
@@ -3249,13 +3249,13 @@
         <v>-6.9118</v>
       </c>
       <c r="D104" t="n">
-        <v>368.608315098468</v>
+        <v>386.401234567901</v>
       </c>
       <c r="E104" t="n">
-        <v>368.608315098468</v>
+        <v>386.401234567901</v>
       </c>
       <c r="F104" t="n">
-        <v>168454</v>
+        <v>187791</v>
       </c>
     </row>
     <row r="105">
@@ -3269,13 +3269,13 @@
         <v>-42.6043</v>
       </c>
       <c r="D105" t="n">
-        <v>16.3676148796499</v>
+        <v>17.2592592592593</v>
       </c>
       <c r="E105" t="n">
-        <v>16.3676148796499</v>
+        <v>17.2592592592593</v>
       </c>
       <c r="F105" t="n">
-        <v>7480</v>
+        <v>8388</v>
       </c>
     </row>
     <row r="106">
@@ -3289,13 +3289,13 @@
         <v>9.5018</v>
       </c>
       <c r="D106" t="n">
-        <v>71799.7658643326</v>
+        <v>82903.4135802469</v>
       </c>
       <c r="E106" t="n">
-        <v>71799.7658643326</v>
+        <v>82903.4135802469</v>
       </c>
       <c r="F106" t="n">
-        <v>32812493</v>
+        <v>40291059</v>
       </c>
     </row>
     <row r="107">
@@ -3309,13 +3309,13 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>673.059080962801</v>
+        <v>675.382716049383</v>
       </c>
       <c r="E107" t="n">
-        <v>673.059080962801</v>
+        <v>675.382716049383</v>
       </c>
       <c r="F107" t="n">
-        <v>307588</v>
+        <v>328236</v>
       </c>
     </row>
     <row r="108">
@@ -3329,13 +3329,13 @@
         <v>42.5903</v>
       </c>
       <c r="D108" t="n">
-        <v>4309.33479212254</v>
+        <v>4722.12757201646</v>
       </c>
       <c r="E108" t="n">
-        <v>4309.33479212254</v>
+        <v>4722.12757201646</v>
       </c>
       <c r="F108" t="n">
-        <v>1969366</v>
+        <v>2294954</v>
       </c>
     </row>
     <row r="109">
@@ -3349,13 +3349,13 @@
         <v>-61.371</v>
       </c>
       <c r="D109" t="n">
-        <v>53.7330415754923</v>
+        <v>61.0308641975309</v>
       </c>
       <c r="E109" t="n">
-        <v>53.7330415754923</v>
+        <v>61.0308641975309</v>
       </c>
       <c r="F109" t="n">
-        <v>24556</v>
+        <v>29661</v>
       </c>
     </row>
     <row r="110">
@@ -3369,13 +3369,13 @@
         <v>-70.1627</v>
       </c>
       <c r="D110" t="n">
-        <v>102512.308533917</v>
+        <v>112572.069958848</v>
       </c>
       <c r="E110" t="n">
-        <v>102512.308533917</v>
+        <v>112572.069958848</v>
       </c>
       <c r="F110" t="n">
-        <v>46848125</v>
+        <v>54710026</v>
       </c>
     </row>
     <row r="111">
@@ -3389,13 +3389,13 @@
         <v>-78.1834</v>
       </c>
       <c r="D111" t="n">
-        <v>131227.087527352</v>
+        <v>146960.934156379</v>
       </c>
       <c r="E111" t="n">
-        <v>131227.087527352</v>
+        <v>146960.934156379</v>
       </c>
       <c r="F111" t="n">
-        <v>59970779</v>
+        <v>71423014</v>
       </c>
     </row>
     <row r="112">
@@ -3409,13 +3409,13 @@
         <v>30.802498</v>
       </c>
       <c r="D112" t="n">
-        <v>90338.5623632385</v>
+        <v>99001.3436213992</v>
       </c>
       <c r="E112" t="n">
-        <v>90338.5623632385</v>
+        <v>99001.3436213992</v>
       </c>
       <c r="F112" t="n">
-        <v>41284723</v>
+        <v>48114653</v>
       </c>
     </row>
     <row r="113">
@@ -3429,13 +3429,13 @@
         <v>-88.8965</v>
       </c>
       <c r="D113" t="n">
-        <v>26268.4332603939</v>
+        <v>28884.4032921811</v>
       </c>
       <c r="E113" t="n">
-        <v>26268.4332603939</v>
+        <v>28884.4032921811</v>
       </c>
       <c r="F113" t="n">
-        <v>12004674</v>
+        <v>14037820</v>
       </c>
     </row>
     <row r="114">
@@ -3449,13 +3449,13 @@
         <v>10.2679</v>
       </c>
       <c r="D114" t="n">
-        <v>3562.80087527352</v>
+        <v>3810.69958847737</v>
       </c>
       <c r="E114" t="n">
-        <v>3562.80087527352</v>
+        <v>3810.69958847737</v>
       </c>
       <c r="F114" t="n">
-        <v>1628200</v>
+        <v>1852000</v>
       </c>
     </row>
     <row r="115">
@@ -3469,13 +3469,13 @@
         <v>39.7823</v>
       </c>
       <c r="D115" t="n">
-        <v>836.92341356674</v>
+        <v>1010.53497942387</v>
       </c>
       <c r="E115" t="n">
-        <v>836.92341356674</v>
+        <v>1010.53497942387</v>
       </c>
       <c r="F115" t="n">
-        <v>382474</v>
+        <v>491120</v>
       </c>
     </row>
     <row r="116">
@@ -3489,13 +3489,13 @@
         <v>25.0136</v>
       </c>
       <c r="D116" t="n">
-        <v>20132.1903719912</v>
+        <v>26344.0288065844</v>
       </c>
       <c r="E116" t="n">
-        <v>20132.1903719912</v>
+        <v>26344.0288065844</v>
       </c>
       <c r="F116" t="n">
-        <v>9200411</v>
+        <v>12803198</v>
       </c>
     </row>
     <row r="117">
@@ -3509,13 +3509,13 @@
         <v>31.4659</v>
       </c>
       <c r="D117" t="n">
-        <v>5944.77899343545</v>
+        <v>6692.8353909465</v>
       </c>
       <c r="E117" t="n">
-        <v>5944.77899343545</v>
+        <v>6692.8353909465</v>
       </c>
       <c r="F117" t="n">
-        <v>2716764</v>
+        <v>3252718</v>
       </c>
     </row>
     <row r="118">
@@ -3529,13 +3529,13 @@
         <v>40.4897</v>
       </c>
       <c r="D118" t="n">
-        <v>69289.7527352298</v>
+        <v>80715.70781893</v>
       </c>
       <c r="E118" t="n">
-        <v>69289.7527352298</v>
+        <v>80715.70781893</v>
       </c>
       <c r="F118" t="n">
-        <v>31665417</v>
+        <v>39227834</v>
       </c>
     </row>
     <row r="119">
@@ -3549,13 +3549,13 @@
         <v>178.065</v>
       </c>
       <c r="D119" t="n">
-        <v>31.6280087527352</v>
+        <v>37.9609053497942</v>
       </c>
       <c r="E119" t="n">
-        <v>31.6280087527352</v>
+        <v>37.9609053497942</v>
       </c>
       <c r="F119" t="n">
-        <v>14454</v>
+        <v>18449</v>
       </c>
     </row>
     <row r="120">
@@ -3569,13 +3569,13 @@
         <v>25.748151</v>
       </c>
       <c r="D120" t="n">
-        <v>21464.9803063457</v>
+        <v>25449.853909465</v>
       </c>
       <c r="E120" t="n">
-        <v>21464.9803063457</v>
+        <v>25449.853909465</v>
       </c>
       <c r="F120" t="n">
-        <v>9809496</v>
+        <v>12368629</v>
       </c>
     </row>
     <row r="121">
@@ -3589,13 +3589,13 @@
         <v>-53.1258</v>
       </c>
       <c r="D121" t="n">
-        <v>7980.21444201313</v>
+        <v>8711.77983539095</v>
       </c>
       <c r="E121" t="n">
-        <v>7980.21444201313</v>
+        <v>8711.77983539095</v>
       </c>
       <c r="F121" t="n">
-        <v>3646958</v>
+        <v>4233925</v>
       </c>
     </row>
     <row r="122">
@@ -3609,13 +3609,13 @@
         <v>149.4068</v>
       </c>
       <c r="D122" t="n">
-        <v>6704.4420131291</v>
+        <v>7425.17489711934</v>
       </c>
       <c r="E122" t="n">
-        <v>6704.4420131291</v>
+        <v>7425.17489711934</v>
       </c>
       <c r="F122" t="n">
-        <v>3063930</v>
+        <v>3608635</v>
       </c>
     </row>
     <row r="123">
@@ -3629,13 +3629,13 @@
         <v>-61.551</v>
       </c>
       <c r="D123" t="n">
-        <v>4348.15754923414</v>
+        <v>4968.96913580247</v>
       </c>
       <c r="E123" t="n">
-        <v>4348.15754923414</v>
+        <v>4968.96913580247</v>
       </c>
       <c r="F123" t="n">
-        <v>1987108</v>
+        <v>2414919</v>
       </c>
     </row>
     <row r="124">
@@ -3649,13 +3649,13 @@
         <v>-61.0242</v>
       </c>
       <c r="D124" t="n">
-        <v>2721.24507658643</v>
+        <v>3218.5987654321</v>
       </c>
       <c r="E124" t="n">
-        <v>2721.24507658643</v>
+        <v>3218.5987654321</v>
       </c>
       <c r="F124" t="n">
-        <v>1243609</v>
+        <v>1564239</v>
       </c>
     </row>
     <row r="125">
@@ -3669,13 +3669,13 @@
         <v>45.166244</v>
       </c>
       <c r="D125" t="n">
-        <v>5330.03282275711</v>
+        <v>6210.52674897119</v>
       </c>
       <c r="E125" t="n">
-        <v>5330.03282275711</v>
+        <v>6210.52674897119</v>
       </c>
       <c r="F125" t="n">
-        <v>2435825</v>
+        <v>3018316</v>
       </c>
     </row>
     <row r="126">
@@ -3689,13 +3689,13 @@
         <v>165.618042</v>
       </c>
       <c r="D126" t="n">
-        <v>33.3610503282276</v>
+        <v>38.7777777777778</v>
       </c>
       <c r="E126" t="n">
-        <v>33.3610503282276</v>
+        <v>38.7777777777778</v>
       </c>
       <c r="F126" t="n">
-        <v>15246</v>
+        <v>18846</v>
       </c>
     </row>
     <row r="127">
@@ -3709,13 +3709,13 @@
         <v>55.5364</v>
       </c>
       <c r="D127" t="n">
-        <v>4893.44420131291</v>
+        <v>5876.72222222222</v>
       </c>
       <c r="E127" t="n">
-        <v>4893.44420131291</v>
+        <v>5876.72222222222</v>
       </c>
       <c r="F127" t="n">
-        <v>2236304</v>
+        <v>2856087</v>
       </c>
     </row>
     <row r="128">
@@ -3729,13 +3729,13 @@
         <v>-62.8333</v>
       </c>
       <c r="D128" t="n">
-        <v>163.752735229759</v>
+        <v>212.06378600823</v>
       </c>
       <c r="E128" t="n">
-        <v>163.752735229759</v>
+        <v>212.06378600823</v>
       </c>
       <c r="F128" t="n">
-        <v>74835</v>
+        <v>103063</v>
       </c>
     </row>
     <row r="129">
@@ -3749,13 +3749,13 @@
         <v>-56.3159</v>
       </c>
       <c r="D129" t="n">
-        <v>9.98249452954048</v>
+        <v>10.8786008230453</v>
       </c>
       <c r="E129" t="n">
-        <v>9.98249452954048</v>
+        <v>10.8786008230453</v>
       </c>
       <c r="F129" t="n">
-        <v>4562</v>
+        <v>5287</v>
       </c>
     </row>
     <row r="130">
@@ -3769,13 +3769,13 @@
         <v>-63.0501</v>
       </c>
       <c r="D130" t="n">
-        <v>522.08533916849</v>
+        <v>596.30658436214</v>
       </c>
       <c r="E130" t="n">
-        <v>522.08533916849</v>
+        <v>596.30658436214</v>
       </c>
       <c r="F130" t="n">
-        <v>238593</v>
+        <v>289805</v>
       </c>
     </row>
     <row r="131">
@@ -3789,13 +3789,13 @@
         <v>-178.1165</v>
       </c>
       <c r="D131" t="n">
-        <v>35.1269146608315</v>
+        <v>59.5246913580247</v>
       </c>
       <c r="E131" t="n">
-        <v>35.1269146608315</v>
+        <v>59.5246913580247</v>
       </c>
       <c r="F131" t="n">
-        <v>16053</v>
+        <v>28929</v>
       </c>
     </row>
     <row r="132">
@@ -3809,13 +3809,13 @@
         <v>2.2137</v>
       </c>
       <c r="D132" t="n">
-        <v>1373214.35448578</v>
+        <v>1629842.83539095</v>
       </c>
       <c r="E132" t="n">
-        <v>1373214.35448578</v>
+        <v>1629842.83539095</v>
       </c>
       <c r="F132" t="n">
-        <v>627558960</v>
+        <v>792103618</v>
       </c>
     </row>
     <row r="133">
@@ -3829,13 +3829,13 @@
         <v>11.6094</v>
       </c>
       <c r="D133" t="n">
-        <v>7369.43544857768</v>
+        <v>8320.68930041152</v>
       </c>
       <c r="E133" t="n">
-        <v>7369.43544857768</v>
+        <v>8320.68930041152</v>
       </c>
       <c r="F133" t="n">
-        <v>3367832</v>
+        <v>4043855</v>
       </c>
     </row>
     <row r="134">
@@ -3849,13 +3849,13 @@
         <v>-15.3101</v>
       </c>
       <c r="D134" t="n">
-        <v>2256.67396061269</v>
+        <v>2474.98353909465</v>
       </c>
       <c r="E134" t="n">
-        <v>2256.67396061269</v>
+        <v>2474.98353909465</v>
       </c>
       <c r="F134" t="n">
-        <v>1031300</v>
+        <v>1202842</v>
       </c>
     </row>
     <row r="135">
@@ -3869,13 +3869,13 @@
         <v>43.3569</v>
       </c>
       <c r="D135" t="n">
-        <v>85823.3960612691</v>
+        <v>99724.512345679</v>
       </c>
       <c r="E135" t="n">
-        <v>85823.3960612691</v>
+        <v>99724.512345679</v>
       </c>
       <c r="F135" t="n">
-        <v>39221292</v>
+        <v>48466113</v>
       </c>
     </row>
     <row r="136">
@@ -3889,13 +3889,13 @@
         <v>10.451526</v>
       </c>
       <c r="D136" t="n">
-        <v>861313.897155361</v>
+        <v>1018100.65432099</v>
       </c>
       <c r="E136" t="n">
-        <v>861313.897155361</v>
+        <v>1018100.65432099</v>
       </c>
       <c r="F136" t="n">
-        <v>393620451</v>
+        <v>494796918</v>
       </c>
     </row>
     <row r="137">
@@ -3909,13 +3909,13 @@
         <v>-1.0232</v>
       </c>
       <c r="D137" t="n">
-        <v>37948.8205689278</v>
+        <v>41224.5308641975</v>
       </c>
       <c r="E137" t="n">
-        <v>37948.8205689278</v>
+        <v>41224.5308641975</v>
       </c>
       <c r="F137" t="n">
-        <v>17342611</v>
+        <v>20035122</v>
       </c>
     </row>
     <row r="138">
@@ -3929,13 +3929,13 @@
         <v>21.8243</v>
       </c>
       <c r="D138" t="n">
-        <v>67742.7439824945</v>
+        <v>85077.7037037037</v>
       </c>
       <c r="E138" t="n">
-        <v>67742.7439824945</v>
+        <v>85077.7037037037</v>
       </c>
       <c r="F138" t="n">
-        <v>30958434</v>
+        <v>41347764</v>
       </c>
     </row>
     <row r="139">
@@ -3949,13 +3949,13 @@
         <v>-61.679</v>
       </c>
       <c r="D139" t="n">
-        <v>54.2800875273523</v>
+        <v>60.59670781893</v>
       </c>
       <c r="E139" t="n">
-        <v>54.2800875273523</v>
+        <v>60.59670781893</v>
       </c>
       <c r="F139" t="n">
-        <v>24806</v>
+        <v>29450</v>
       </c>
     </row>
     <row r="140">
@@ -3969,13 +3969,13 @@
         <v>-90.2308</v>
       </c>
       <c r="D140" t="n">
-        <v>78807.9080962801</v>
+        <v>88014.9917695473</v>
       </c>
       <c r="E140" t="n">
-        <v>78807.9080962801</v>
+        <v>88014.9917695473</v>
       </c>
       <c r="F140" t="n">
-        <v>36015214</v>
+        <v>42775286</v>
       </c>
     </row>
     <row r="141">
@@ -3989,13 +3989,13 @@
         <v>-9.6966</v>
       </c>
       <c r="D141" t="n">
-        <v>8806.5010940919</v>
+        <v>9621.99382716049</v>
       </c>
       <c r="E141" t="n">
-        <v>8806.5010940919</v>
+        <v>9621.99382716049</v>
       </c>
       <c r="F141" t="n">
-        <v>4024571</v>
+        <v>4676289</v>
       </c>
     </row>
     <row r="142">
@@ -4009,13 +4009,13 @@
         <v>-15.1804</v>
       </c>
       <c r="D142" t="n">
-        <v>1827.69803063457</v>
+        <v>1941.68930041152</v>
       </c>
       <c r="E142" t="n">
-        <v>1827.69803063457</v>
+        <v>1941.68930041152</v>
       </c>
       <c r="F142" t="n">
-        <v>835258</v>
+        <v>943661</v>
       </c>
     </row>
     <row r="143">
@@ -4029,13 +4029,13 @@
         <v>-58.93018</v>
       </c>
       <c r="D143" t="n">
-        <v>3343.46608315098</v>
+        <v>3985.62962962963</v>
       </c>
       <c r="E143" t="n">
-        <v>3343.46608315098</v>
+        <v>3985.62962962963</v>
       </c>
       <c r="F143" t="n">
-        <v>1527964</v>
+        <v>1937016</v>
       </c>
     </row>
     <row r="144">
@@ -4049,13 +4049,13 @@
         <v>-72.2852</v>
       </c>
       <c r="D144" t="n">
-        <v>6649.16411378556</v>
+        <v>7039.88477366255</v>
       </c>
       <c r="E144" t="n">
-        <v>6649.16411378556</v>
+        <v>7039.88477366255</v>
       </c>
       <c r="F144" t="n">
-        <v>3038668</v>
+        <v>3421384</v>
       </c>
     </row>
     <row r="145">
@@ -4069,13 +4069,13 @@
         <v>12.4534</v>
       </c>
       <c r="D145" t="n">
-        <v>16.308533916849</v>
+        <v>16.9465020576132</v>
       </c>
       <c r="E145" t="n">
-        <v>16.308533916849</v>
+        <v>16.9465020576132</v>
       </c>
       <c r="F145" t="n">
-        <v>7453</v>
+        <v>8236</v>
       </c>
     </row>
     <row r="146">
@@ -4089,13 +4089,13 @@
         <v>-86.2419</v>
       </c>
       <c r="D146" t="n">
-        <v>72075.8358862144</v>
+        <v>80787.7201646091</v>
       </c>
       <c r="E146" t="n">
-        <v>72075.8358862144</v>
+        <v>80787.7201646091</v>
       </c>
       <c r="F146" t="n">
-        <v>32938657</v>
+        <v>39262832</v>
       </c>
     </row>
     <row r="147">
@@ -4109,13 +4109,13 @@
         <v>19.5033</v>
       </c>
       <c r="D147" t="n">
-        <v>152433.787746171</v>
+        <v>190290.477366255</v>
       </c>
       <c r="E147" t="n">
-        <v>152433.787746171</v>
+        <v>190290.477366255</v>
       </c>
       <c r="F147" t="n">
-        <v>69662241</v>
+        <v>92481172</v>
       </c>
     </row>
     <row r="148">
@@ -4129,13 +4129,13 @@
         <v>-19.0208</v>
       </c>
       <c r="D148" t="n">
-        <v>3254.93216630197</v>
+        <v>3448.22839506173</v>
       </c>
       <c r="E148" t="n">
-        <v>3254.93216630197</v>
+        <v>3448.22839506173</v>
       </c>
       <c r="F148" t="n">
-        <v>1487504</v>
+        <v>1675839</v>
       </c>
     </row>
     <row r="149">
@@ -4149,13 +4149,13 @@
         <v>78.96288</v>
       </c>
       <c r="D149" t="n">
-        <v>5206603.31509847</v>
+        <v>6191390.4218107</v>
       </c>
       <c r="E149" t="n">
-        <v>5206603.31509847</v>
+        <v>6191390.4218107</v>
       </c>
       <c r="F149" t="n">
-        <v>2379417715</v>
+        <v>3009015745</v>
       </c>
     </row>
     <row r="150">
@@ -4169,13 +4169,13 @@
         <v>113.9213</v>
       </c>
       <c r="D150" t="n">
-        <v>441045.754923414</v>
+        <v>516184.820987654</v>
       </c>
       <c r="E150" t="n">
-        <v>441045.754923414</v>
+        <v>516184.820987654</v>
       </c>
       <c r="F150" t="n">
-        <v>201557910</v>
+        <v>250865823</v>
       </c>
     </row>
     <row r="151">
@@ -4189,13 +4189,13 @@
         <v>53.688046</v>
       </c>
       <c r="D151" t="n">
-        <v>661543.658643326</v>
+        <v>777846.508230453</v>
       </c>
       <c r="E151" t="n">
-        <v>661543.658643326</v>
+        <v>777846.508230453</v>
       </c>
       <c r="F151" t="n">
-        <v>302325452</v>
+        <v>378033403</v>
       </c>
     </row>
     <row r="152">
@@ -4209,13 +4209,13 @@
         <v>43.679291</v>
       </c>
       <c r="D152" t="n">
-        <v>319579.15536105</v>
+        <v>366003.222222222</v>
       </c>
       <c r="E152" t="n">
-        <v>319579.15536105</v>
+        <v>366003.222222222</v>
       </c>
       <c r="F152" t="n">
-        <v>146047674</v>
+        <v>177877566</v>
       </c>
     </row>
     <row r="153">
@@ -4229,13 +4229,13 @@
         <v>-7.6921</v>
       </c>
       <c r="D153" t="n">
-        <v>73617.0240700219</v>
+        <v>84228.7325102881</v>
       </c>
       <c r="E153" t="n">
-        <v>73617.0240700219</v>
+        <v>84228.7325102881</v>
       </c>
       <c r="F153" t="n">
-        <v>33642980</v>
+        <v>40935164</v>
       </c>
     </row>
     <row r="154">
@@ -4249,13 +4249,13 @@
         <v>34.851612</v>
       </c>
       <c r="D154" t="n">
-        <v>267445.24726477</v>
+        <v>301534.878600823</v>
       </c>
       <c r="E154" t="n">
-        <v>267445.24726477</v>
+        <v>301534.878600823</v>
       </c>
       <c r="F154" t="n">
-        <v>122222478</v>
+        <v>146545951</v>
       </c>
     </row>
     <row r="155">
@@ -4269,13 +4269,13 @@
         <v>12.56738</v>
       </c>
       <c r="D155" t="n">
-        <v>1060794.23413567</v>
+        <v>1240933.04526749</v>
       </c>
       <c r="E155" t="n">
-        <v>1060794.23413567</v>
+        <v>1240933.04526749</v>
       </c>
       <c r="F155" t="n">
-        <v>484782965</v>
+        <v>603093460</v>
       </c>
     </row>
     <row r="156">
@@ -4289,13 +4289,13 @@
         <v>-77.2975</v>
       </c>
       <c r="D156" t="n">
-        <v>8852.4113785558</v>
+        <v>11090.2757201646</v>
       </c>
       <c r="E156" t="n">
-        <v>8852.4113785558</v>
+        <v>11090.2757201646</v>
       </c>
       <c r="F156" t="n">
-        <v>4045552</v>
+        <v>5389874</v>
       </c>
     </row>
     <row r="157">
@@ -4309,13 +4309,13 @@
         <v>138.252924</v>
       </c>
       <c r="D157" t="n">
-        <v>142704.286652079</v>
+        <v>171931.37037037</v>
       </c>
       <c r="E157" t="n">
-        <v>142704.286652079</v>
+        <v>171931.37037037</v>
       </c>
       <c r="F157" t="n">
-        <v>65215859</v>
+        <v>83558646</v>
       </c>
     </row>
     <row r="158">
@@ -4329,13 +4329,13 @@
         <v>36.51</v>
       </c>
       <c r="D158" t="n">
-        <v>139424</v>
+        <v>173855.493827161</v>
       </c>
       <c r="E158" t="n">
-        <v>139424</v>
+        <v>173855.493827161</v>
       </c>
       <c r="F158" t="n">
-        <v>63716768</v>
+        <v>84493770</v>
       </c>
     </row>
     <row r="159">
@@ -4349,13 +4349,13 @@
         <v>66.9237</v>
       </c>
       <c r="D159" t="n">
-        <v>120828.72428884</v>
+        <v>137013.646090535</v>
       </c>
       <c r="E159" t="n">
-        <v>120828.72428884</v>
+        <v>137013.646090535</v>
       </c>
       <c r="F159" t="n">
-        <v>55218727</v>
+        <v>66588632</v>
       </c>
     </row>
     <row r="160">
@@ -4369,13 +4369,13 @@
         <v>37.9062</v>
       </c>
       <c r="D160" t="n">
-        <v>47431.010940919</v>
+        <v>54269.6728395062</v>
       </c>
       <c r="E160" t="n">
-        <v>47431.010940919</v>
+        <v>54269.6728395062</v>
       </c>
       <c r="F160" t="n">
-        <v>21675972</v>
+        <v>26375061</v>
       </c>
     </row>
     <row r="161">
@@ -4389,13 +4389,13 @@
         <v>127.766922</v>
       </c>
       <c r="D161" t="n">
-        <v>35088.886214442</v>
+        <v>40557.4814814815</v>
       </c>
       <c r="E161" t="n">
-        <v>35088.886214442</v>
+        <v>40557.4814814815</v>
       </c>
       <c r="F161" t="n">
-        <v>16035621</v>
+        <v>19710936</v>
       </c>
     </row>
     <row r="162">
@@ -4409,13 +4409,13 @@
         <v>20.902977</v>
       </c>
       <c r="D162" t="n">
-        <v>26225.7439824945</v>
+        <v>30926.3004115226</v>
       </c>
       <c r="E162" t="n">
-        <v>26225.7439824945</v>
+        <v>30926.3004115226</v>
       </c>
       <c r="F162" t="n">
-        <v>11985165</v>
+        <v>15030182</v>
       </c>
     </row>
     <row r="163">
@@ -4429,13 +4429,13 @@
         <v>47.481766</v>
       </c>
       <c r="D163" t="n">
-        <v>93544.1181619256</v>
+        <v>104777.705761317</v>
       </c>
       <c r="E163" t="n">
-        <v>93544.1181619256</v>
+        <v>104777.705761317</v>
       </c>
       <c r="F163" t="n">
-        <v>42749662</v>
+        <v>50921965</v>
       </c>
     </row>
     <row r="164">
@@ -4449,13 +4449,13 @@
         <v>74.766098</v>
       </c>
       <c r="D164" t="n">
-        <v>41652.8205689278</v>
+        <v>44991.4691358025</v>
       </c>
       <c r="E164" t="n">
-        <v>41652.8205689278</v>
+        <v>44991.4691358025</v>
       </c>
       <c r="F164" t="n">
-        <v>19035339</v>
+        <v>21865854</v>
       </c>
     </row>
     <row r="165">
@@ -4469,13 +4469,13 @@
         <v>102.495496</v>
       </c>
       <c r="D165" t="n">
-        <v>25.6673960612691</v>
+        <v>90.5288065843621</v>
       </c>
       <c r="E165" t="n">
-        <v>25.6673960612691</v>
+        <v>90.5288065843621</v>
       </c>
       <c r="F165" t="n">
-        <v>11730</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="166">
@@ -4489,13 +4489,13 @@
         <v>24.6032</v>
       </c>
       <c r="D166" t="n">
-        <v>23327.9671772429</v>
+        <v>29243.1728395062</v>
       </c>
       <c r="E166" t="n">
-        <v>23327.9671772429</v>
+        <v>29243.1728395062</v>
       </c>
       <c r="F166" t="n">
-        <v>10660881</v>
+        <v>14212182</v>
       </c>
     </row>
     <row r="167">
@@ -4509,13 +4509,13 @@
         <v>35.8623</v>
       </c>
       <c r="D167" t="n">
-        <v>114210.807439825</v>
+        <v>139038.543209877</v>
       </c>
       <c r="E167" t="n">
-        <v>114210.807439825</v>
+        <v>139038.543209877</v>
       </c>
       <c r="F167" t="n">
-        <v>52194339</v>
+        <v>67572732</v>
       </c>
     </row>
     <row r="168">
@@ -4529,13 +4529,13 @@
         <v>28.2336</v>
       </c>
       <c r="D168" t="n">
-        <v>2859.15317286652</v>
+        <v>3330.50205761317</v>
       </c>
       <c r="E168" t="n">
-        <v>2859.15317286652</v>
+        <v>3330.50205761317</v>
       </c>
       <c r="F168" t="n">
-        <v>1306633</v>
+        <v>1618624</v>
       </c>
     </row>
     <row r="169">
@@ -4549,13 +4549,13 @@
         <v>-9.429499</v>
       </c>
       <c r="D169" t="n">
-        <v>1089.31947483589</v>
+        <v>1150.32510288066</v>
       </c>
       <c r="E169" t="n">
-        <v>1089.31947483589</v>
+        <v>1150.32510288066</v>
       </c>
       <c r="F169" t="n">
-        <v>497819</v>
+        <v>559058</v>
       </c>
     </row>
     <row r="170">
@@ -4569,13 +4569,13 @@
         <v>17.228331</v>
       </c>
       <c r="D170" t="n">
-        <v>49868.0371991247</v>
+        <v>57584.5164609053</v>
       </c>
       <c r="E170" t="n">
-        <v>49868.0371991247</v>
+        <v>57584.5164609053</v>
       </c>
       <c r="F170" t="n">
-        <v>22789693</v>
+        <v>27986075</v>
       </c>
     </row>
     <row r="171">
@@ -4589,13 +4589,13 @@
         <v>9.55</v>
       </c>
       <c r="D171" t="n">
-        <v>855.768052516411</v>
+        <v>980.748971193416</v>
       </c>
       <c r="E171" t="n">
-        <v>855.768052516411</v>
+        <v>980.748971193416</v>
       </c>
       <c r="F171" t="n">
-        <v>391086</v>
+        <v>476644</v>
       </c>
     </row>
     <row r="172">
@@ -4609,13 +4609,13 @@
         <v>23.8813</v>
       </c>
       <c r="D172" t="n">
-        <v>58574.7943107221</v>
+        <v>70295.6111111111</v>
       </c>
       <c r="E172" t="n">
-        <v>58574.7943107221</v>
+        <v>70295.6111111111</v>
       </c>
       <c r="F172" t="n">
-        <v>26768681</v>
+        <v>34163667</v>
       </c>
     </row>
     <row r="173">
@@ -4629,13 +4629,13 @@
         <v>6.1296</v>
       </c>
       <c r="D173" t="n">
-        <v>21065.4442013129</v>
+        <v>23861.9979423868</v>
       </c>
       <c r="E173" t="n">
-        <v>21065.4442013129</v>
+        <v>23861.9979423868</v>
       </c>
       <c r="F173" t="n">
-        <v>9626908</v>
+        <v>11596931</v>
       </c>
     </row>
     <row r="174">
@@ -4649,13 +4649,13 @@
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>7.63894967177243</v>
+        <v>7.7201646090535</v>
       </c>
       <c r="E174" t="n">
-        <v>7.63894967177243</v>
+        <v>7.7201646090535</v>
       </c>
       <c r="F174" t="n">
-        <v>3491</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="175">
@@ -4669,13 +4669,13 @@
         <v>46.869107</v>
       </c>
       <c r="D175" t="n">
-        <v>11245.7330415755</v>
+        <v>12862.3991769547</v>
       </c>
       <c r="E175" t="n">
-        <v>11245.7330415755</v>
+        <v>12862.3991769547</v>
       </c>
       <c r="F175" t="n">
-        <v>5139300</v>
+        <v>6251126</v>
       </c>
     </row>
     <row r="176">
@@ -4689,13 +4689,13 @@
         <v>34.3015</v>
       </c>
       <c r="D176" t="n">
-        <v>8688.71991247265</v>
+        <v>10207.353909465</v>
       </c>
       <c r="E176" t="n">
-        <v>8688.71991247265</v>
+        <v>10207.353909465</v>
       </c>
       <c r="F176" t="n">
-        <v>3970745</v>
+        <v>4960774</v>
       </c>
     </row>
     <row r="177">
@@ -4709,13 +4709,13 @@
         <v>101.975766</v>
       </c>
       <c r="D177" t="n">
-        <v>80222.9978118162</v>
+        <v>101445.633744856</v>
       </c>
       <c r="E177" t="n">
-        <v>80222.9978118162</v>
+        <v>101445.633744856</v>
       </c>
       <c r="F177" t="n">
-        <v>36661910</v>
+        <v>49302578</v>
       </c>
     </row>
     <row r="178">
@@ -4729,13 +4729,13 @@
         <v>73.2207</v>
       </c>
       <c r="D178" t="n">
-        <v>8697.78118161926</v>
+        <v>10351.8333333333</v>
       </c>
       <c r="E178" t="n">
-        <v>8697.78118161926</v>
+        <v>10351.8333333333</v>
       </c>
       <c r="F178" t="n">
-        <v>3974886</v>
+        <v>5030991</v>
       </c>
     </row>
     <row r="179">
@@ -4749,13 +4749,13 @@
         <v>-3.996166</v>
       </c>
       <c r="D179" t="n">
-        <v>3837.75711159737</v>
+        <v>4443.47942386831</v>
       </c>
       <c r="E179" t="n">
-        <v>3837.75711159737</v>
+        <v>4443.47942386831</v>
       </c>
       <c r="F179" t="n">
-        <v>1753855</v>
+        <v>2159531</v>
       </c>
     </row>
     <row r="180">
@@ -4769,13 +4769,13 @@
         <v>14.3754</v>
       </c>
       <c r="D180" t="n">
-        <v>7508.00218818381</v>
+        <v>8872.63580246914</v>
       </c>
       <c r="E180" t="n">
-        <v>7508.00218818381</v>
+        <v>8872.63580246914</v>
       </c>
       <c r="F180" t="n">
-        <v>3431157</v>
+        <v>4312101</v>
       </c>
     </row>
     <row r="181">
@@ -4789,13 +4789,13 @@
         <v>171.1845</v>
       </c>
       <c r="D181" t="n">
-        <v>1.43544857768053</v>
+        <v>1.58847736625514</v>
       </c>
       <c r="E181" t="n">
-        <v>1.43544857768053</v>
+        <v>1.58847736625514</v>
       </c>
       <c r="F181" t="n">
-        <v>656</v>
+        <v>772</v>
       </c>
     </row>
     <row r="182">
@@ -4809,13 +4809,13 @@
         <v>-10.9408</v>
       </c>
       <c r="D182" t="n">
-        <v>7464.44857768052</v>
+        <v>8128.92386831276</v>
       </c>
       <c r="E182" t="n">
-        <v>7464.44857768052</v>
+        <v>8128.92386831276</v>
       </c>
       <c r="F182" t="n">
-        <v>3411253</v>
+        <v>3950657</v>
       </c>
     </row>
     <row r="183">
@@ -4829,13 +4829,13 @@
         <v>57.552152</v>
       </c>
       <c r="D183" t="n">
-        <v>413.01750547046</v>
+        <v>462.40329218107</v>
       </c>
       <c r="E183" t="n">
-        <v>413.01750547046</v>
+        <v>462.40329218107</v>
       </c>
       <c r="F183" t="n">
-        <v>188749</v>
+        <v>224728</v>
       </c>
     </row>
     <row r="184">
@@ -4849,13 +4849,13 @@
         <v>-102.5528</v>
       </c>
       <c r="D184" t="n">
-        <v>815810.207877462</v>
+        <v>907934.987654321</v>
       </c>
       <c r="E184" t="n">
-        <v>815810.207877462</v>
+        <v>907934.987654321</v>
       </c>
       <c r="F184" t="n">
-        <v>372825265</v>
+        <v>441256404</v>
       </c>
     </row>
     <row r="185">
@@ -4869,13 +4869,13 @@
         <v>150.5508</v>
       </c>
       <c r="D185" t="n">
-        <v>0.201312910284464</v>
+        <v>0.248971193415638</v>
       </c>
       <c r="E185" t="n">
-        <v>0.201312910284464</v>
+        <v>0.248971193415638</v>
       </c>
       <c r="F185" t="n">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="186">
@@ -4889,13 +4889,13 @@
         <v>28.3699</v>
       </c>
       <c r="D186" t="n">
-        <v>73435.636761488</v>
+        <v>84092.4135802469</v>
       </c>
       <c r="E186" t="n">
-        <v>73435.636761488</v>
+        <v>84092.4135802469</v>
       </c>
       <c r="F186" t="n">
-        <v>33560086</v>
+        <v>40868913</v>
       </c>
     </row>
     <row r="187">
@@ -4909,13 +4909,13 @@
         <v>7.4167</v>
       </c>
       <c r="D187" t="n">
-        <v>596.921225382932</v>
+        <v>708.738683127572</v>
       </c>
       <c r="E187" t="n">
-        <v>596.921225382932</v>
+        <v>708.738683127572</v>
       </c>
       <c r="F187" t="n">
-        <v>272793</v>
+        <v>344447</v>
       </c>
     </row>
     <row r="188">
@@ -4929,13 +4929,13 @@
         <v>103.8467</v>
       </c>
       <c r="D188" t="n">
-        <v>1587.50547045952</v>
+        <v>4014.58230452675</v>
       </c>
       <c r="E188" t="n">
-        <v>1587.50547045952</v>
+        <v>4014.58230452675</v>
       </c>
       <c r="F188" t="n">
-        <v>725490</v>
+        <v>1951087</v>
       </c>
     </row>
     <row r="189">
@@ -4949,13 +4949,13 @@
         <v>19.37439</v>
       </c>
       <c r="D189" t="n">
-        <v>24843.0590809628</v>
+        <v>29207.8271604938</v>
       </c>
       <c r="E189" t="n">
-        <v>24843.0590809628</v>
+        <v>29207.8271604938</v>
       </c>
       <c r="F189" t="n">
-        <v>11353278</v>
+        <v>14195004</v>
       </c>
     </row>
     <row r="190">
@@ -4969,13 +4969,13 @@
         <v>-7.0926</v>
       </c>
       <c r="D190" t="n">
-        <v>187181.735229759</v>
+        <v>206616.271604938</v>
       </c>
       <c r="E190" t="n">
-        <v>187181.735229759</v>
+        <v>206616.271604938</v>
       </c>
       <c r="F190" t="n">
-        <v>85542053</v>
+        <v>100415508</v>
       </c>
     </row>
     <row r="191">
@@ -4989,13 +4989,13 @@
         <v>35.529562</v>
       </c>
       <c r="D191" t="n">
-        <v>16149.52297593</v>
+        <v>19370.0720164609</v>
       </c>
       <c r="E191" t="n">
-        <v>16149.52297593</v>
+        <v>19370.0720164609</v>
       </c>
       <c r="F191" t="n">
-        <v>7380332</v>
+        <v>9413855</v>
       </c>
     </row>
     <row r="192">
@@ -5009,13 +5009,13 @@
         <v>18.4904</v>
       </c>
       <c r="D192" t="n">
-        <v>13224.7921225383</v>
+        <v>15398.975308642</v>
       </c>
       <c r="E192" t="n">
-        <v>13224.7921225383</v>
+        <v>15398.975308642</v>
       </c>
       <c r="F192" t="n">
-        <v>6043730</v>
+        <v>7483902</v>
       </c>
     </row>
     <row r="193">
@@ -5029,13 +5029,13 @@
         <v>84.25</v>
       </c>
       <c r="D193" t="n">
-        <v>113535.702407002</v>
+        <v>129637.314814815</v>
       </c>
       <c r="E193" t="n">
-        <v>113535.702407002</v>
+        <v>129637.314814815</v>
       </c>
       <c r="F193" t="n">
-        <v>51885816</v>
+        <v>63003735</v>
       </c>
     </row>
     <row r="194">
@@ -5049,13 +5049,13 @@
         <v>-69.9683</v>
       </c>
       <c r="D194" t="n">
-        <v>3200.56455142232</v>
+        <v>3649.63580246914</v>
       </c>
       <c r="E194" t="n">
-        <v>3200.56455142232</v>
+        <v>3649.63580246914</v>
       </c>
       <c r="F194" t="n">
-        <v>1462658</v>
+        <v>1773723</v>
       </c>
     </row>
     <row r="195">
@@ -5069,13 +5069,13 @@
         <v>-68.2385</v>
       </c>
       <c r="D195" t="n">
-        <v>85.4048140043764</v>
+        <v>157.565843621399</v>
       </c>
       <c r="E195" t="n">
-        <v>85.4048140043764</v>
+        <v>157.565843621399</v>
       </c>
       <c r="F195" t="n">
-        <v>39030</v>
+        <v>76577</v>
       </c>
     </row>
     <row r="196">
@@ -5089,13 +5089,13 @@
         <v>-68.99</v>
       </c>
       <c r="D196" t="n">
-        <v>1918.71334792123</v>
+        <v>2532.7304526749</v>
       </c>
       <c r="E196" t="n">
-        <v>1918.71334792123</v>
+        <v>2532.7304526749</v>
       </c>
       <c r="F196" t="n">
-        <v>876852</v>
+        <v>1230907</v>
       </c>
     </row>
     <row r="197">
@@ -5109,13 +5109,13 @@
         <v>-63.0548</v>
       </c>
       <c r="D197" t="n">
-        <v>756.809628008753</v>
+        <v>846.442386831276</v>
       </c>
       <c r="E197" t="n">
-        <v>756.809628008753</v>
+        <v>846.442386831276</v>
       </c>
       <c r="F197" t="n">
-        <v>345862</v>
+        <v>411371</v>
       </c>
     </row>
     <row r="198">
@@ -5129,13 +5129,13 @@
         <v>5.2913</v>
       </c>
       <c r="D198" t="n">
-        <v>379652.884026258</v>
+        <v>448932.664609054</v>
       </c>
       <c r="E198" t="n">
-        <v>379652.884026258</v>
+        <v>448932.664609054</v>
       </c>
       <c r="F198" t="n">
-        <v>173501368</v>
+        <v>218181275</v>
       </c>
     </row>
     <row r="199">
@@ -5149,13 +5149,13 @@
         <v>174.886</v>
       </c>
       <c r="D199" t="n">
-        <v>1616.13566739606</v>
+        <v>1676.79835390947</v>
       </c>
       <c r="E199" t="n">
-        <v>1616.13566739606</v>
+        <v>1676.79835390947</v>
       </c>
       <c r="F199" t="n">
-        <v>738574</v>
+        <v>814924</v>
       </c>
     </row>
     <row r="200">
@@ -5169,13 +5169,13 @@
         <v>-85.207229</v>
       </c>
       <c r="D200" t="n">
-        <v>3651.11597374179</v>
+        <v>3850.78806584362</v>
       </c>
       <c r="E200" t="n">
-        <v>3651.11597374179</v>
+        <v>3850.78806584362</v>
       </c>
       <c r="F200" t="n">
-        <v>1668560</v>
+        <v>1871483</v>
       </c>
     </row>
     <row r="201">
@@ -5189,13 +5189,13 @@
         <v>8.081666</v>
       </c>
       <c r="D201" t="n">
-        <v>1861.50547045952</v>
+        <v>2065.6316872428</v>
       </c>
       <c r="E201" t="n">
-        <v>1861.50547045952</v>
+        <v>2065.6316872428</v>
       </c>
       <c r="F201" t="n">
-        <v>850708</v>
+        <v>1003897</v>
       </c>
     </row>
     <row r="202">
@@ -5209,13 +5209,13 @@
         <v>8.6753</v>
       </c>
       <c r="D202" t="n">
-        <v>59702.829321663</v>
+        <v>66005.9958847737</v>
       </c>
       <c r="E202" t="n">
-        <v>59702.829321663</v>
+        <v>66005.9958847737</v>
       </c>
       <c r="F202" t="n">
-        <v>27284193</v>
+        <v>32078914</v>
       </c>
     </row>
     <row r="203">
@@ -5229,13 +5229,13 @@
         <v>21.7453</v>
       </c>
       <c r="D203" t="n">
-        <v>39313.7571115974</v>
+        <v>46109.183127572</v>
       </c>
       <c r="E203" t="n">
-        <v>39313.7571115974</v>
+        <v>46109.183127572</v>
       </c>
       <c r="F203" t="n">
-        <v>17966387</v>
+        <v>22409063</v>
       </c>
     </row>
     <row r="204">
@@ -5249,13 +5249,13 @@
         <v>8.4689</v>
       </c>
       <c r="D204" t="n">
-        <v>28318.0525164114</v>
+        <v>33531.9115226337</v>
       </c>
       <c r="E204" t="n">
-        <v>28318.0525164114</v>
+        <v>33531.9115226337</v>
       </c>
       <c r="F204" t="n">
-        <v>12941350</v>
+        <v>16296509</v>
       </c>
     </row>
     <row r="205">
@@ -5269,13 +5269,13 @@
         <v>55.923255</v>
       </c>
       <c r="D205" t="n">
-        <v>77403.4070021882</v>
+        <v>84639.0596707819</v>
       </c>
       <c r="E205" t="n">
-        <v>77403.4070021882</v>
+        <v>84639.0596707819</v>
       </c>
       <c r="F205" t="n">
-        <v>35373357</v>
+        <v>41134583</v>
       </c>
     </row>
     <row r="206">
@@ -5289,13 +5289,13 @@
         <v>69.3451</v>
       </c>
       <c r="D206" t="n">
-        <v>292725.964989059</v>
+        <v>325930.674897119</v>
       </c>
       <c r="E206" t="n">
-        <v>292725.964989059</v>
+        <v>325930.674897119</v>
       </c>
       <c r="F206" t="n">
-        <v>133775766</v>
+        <v>158402308</v>
       </c>
     </row>
     <row r="207">
@@ -5309,13 +5309,13 @@
         <v>-80.7821</v>
       </c>
       <c r="D207" t="n">
-        <v>130836.827133479</v>
+        <v>144942.393004115</v>
       </c>
       <c r="E207" t="n">
-        <v>130836.827133479</v>
+        <v>144942.393004115</v>
       </c>
       <c r="F207" t="n">
-        <v>59792430</v>
+        <v>70442003</v>
       </c>
     </row>
     <row r="208">
@@ -5329,13 +5329,13 @@
         <v>143.95555</v>
       </c>
       <c r="D208" t="n">
-        <v>899.006564551422</v>
+        <v>1572.01440329218</v>
       </c>
       <c r="E208" t="n">
-        <v>899.006564551422</v>
+        <v>1572.01440329218</v>
       </c>
       <c r="F208" t="n">
-        <v>410846</v>
+        <v>763999</v>
       </c>
     </row>
     <row r="209">
@@ -5349,13 +5349,13 @@
         <v>-58.4438</v>
       </c>
       <c r="D209" t="n">
-        <v>59028.398249453</v>
+        <v>73048.1913580247</v>
       </c>
       <c r="E209" t="n">
-        <v>59028.398249453</v>
+        <v>73048.1913580247</v>
       </c>
       <c r="F209" t="n">
-        <v>26975978</v>
+        <v>35501421</v>
       </c>
     </row>
     <row r="210">
@@ -5369,13 +5369,13 @@
         <v>-75.0152</v>
       </c>
       <c r="D210" t="n">
-        <v>640112.008752735</v>
+        <v>711282.582304527</v>
       </c>
       <c r="E210" t="n">
-        <v>640112.008752735</v>
+        <v>711282.582304527</v>
       </c>
       <c r="F210" t="n">
-        <v>292531188</v>
+        <v>345683335</v>
       </c>
     </row>
     <row r="211">
@@ -5389,13 +5389,13 @@
         <v>121.774017</v>
       </c>
       <c r="D211" t="n">
-        <v>270123.234135667</v>
+        <v>318660.327160494</v>
       </c>
       <c r="E211" t="n">
-        <v>270123.234135667</v>
+        <v>318660.327160494</v>
       </c>
       <c r="F211" t="n">
-        <v>123446318</v>
+        <v>154868919</v>
       </c>
     </row>
     <row r="212">
@@ -5409,13 +5409,13 @@
         <v>19.1451</v>
       </c>
       <c r="D212" t="n">
-        <v>604059.207877462</v>
+        <v>736084.839506173</v>
       </c>
       <c r="E212" t="n">
-        <v>604059.207877462</v>
+        <v>736084.839506173</v>
       </c>
       <c r="F212" t="n">
-        <v>276055058</v>
+        <v>357737232</v>
       </c>
     </row>
     <row r="213">
@@ -5429,13 +5429,13 @@
         <v>-8.2245</v>
       </c>
       <c r="D213" t="n">
-        <v>242594.807439825</v>
+        <v>278172.911522634</v>
       </c>
       <c r="E213" t="n">
-        <v>242594.807439825</v>
+        <v>278172.911522634</v>
       </c>
       <c r="F213" t="n">
-        <v>110865827</v>
+        <v>135192035</v>
       </c>
     </row>
     <row r="214">
@@ -5449,13 +5449,13 @@
         <v>51.1839</v>
       </c>
       <c r="D214" t="n">
-        <v>98468.1356673961</v>
+        <v>105066.146090535</v>
       </c>
       <c r="E214" t="n">
-        <v>98468.1356673961</v>
+        <v>105066.146090535</v>
       </c>
       <c r="F214" t="n">
-        <v>44999938</v>
+        <v>51062147</v>
       </c>
     </row>
     <row r="215">
@@ -5469,13 +5469,13 @@
         <v>24.9668</v>
       </c>
       <c r="D215" t="n">
-        <v>292505.905908096</v>
+        <v>338420.024691358</v>
       </c>
       <c r="E215" t="n">
-        <v>292505.905908096</v>
+        <v>338420.024691358</v>
       </c>
       <c r="F215" t="n">
-        <v>133675199</v>
+        <v>164472132</v>
       </c>
     </row>
     <row r="216">
@@ -5489,13 +5489,13 @@
         <v>105.318756</v>
       </c>
       <c r="D216" t="n">
-        <v>1644149.52297593</v>
+        <v>1832981.51851852</v>
       </c>
       <c r="E216" t="n">
-        <v>1644149.52297593</v>
+        <v>1832981.51851852</v>
       </c>
       <c r="F216" t="n">
-        <v>751376332</v>
+        <v>890829018</v>
       </c>
     </row>
     <row r="217">
@@ -5509,13 +5509,13 @@
         <v>29.8739</v>
       </c>
       <c r="D217" t="n">
-        <v>6160.26258205689</v>
+        <v>7316.44855967078</v>
       </c>
       <c r="E217" t="n">
-        <v>6160.26258205689</v>
+        <v>7316.44855967078</v>
       </c>
       <c r="F217" t="n">
-        <v>2815240</v>
+        <v>3555794</v>
       </c>
     </row>
     <row r="218">
@@ -5529,13 +5529,13 @@
         <v>-62.782998</v>
       </c>
       <c r="D218" t="n">
-        <v>20.6477024070022</v>
+        <v>22.0884773662551</v>
       </c>
       <c r="E218" t="n">
-        <v>20.6477024070022</v>
+        <v>22.0884773662551</v>
       </c>
       <c r="F218" t="n">
-        <v>9436</v>
+        <v>10735</v>
       </c>
     </row>
     <row r="219">
@@ -5549,13 +5549,13 @@
         <v>-60.9789</v>
       </c>
       <c r="D219" t="n">
-        <v>717.862144420131</v>
+        <v>952.979423868313</v>
       </c>
       <c r="E219" t="n">
-        <v>717.862144420131</v>
+        <v>952.979423868313</v>
       </c>
       <c r="F219" t="n">
-        <v>328063</v>
+        <v>463148</v>
       </c>
     </row>
     <row r="220">
@@ -5569,13 +5569,13 @@
         <v>-61.2872</v>
       </c>
       <c r="D220" t="n">
-        <v>346.98249452954</v>
+        <v>439.405349794239</v>
       </c>
       <c r="E220" t="n">
-        <v>346.98249452954</v>
+        <v>439.405349794239</v>
       </c>
       <c r="F220" t="n">
-        <v>158571</v>
+        <v>213551</v>
       </c>
     </row>
     <row r="221">
@@ -5589,13 +5589,13 @@
         <v>-172.1046</v>
       </c>
       <c r="D221" t="n">
-        <v>0.809628008752735</v>
+        <v>0.940329218106996</v>
       </c>
       <c r="E221" t="n">
-        <v>0.809628008752735</v>
+        <v>0.940329218106996</v>
       </c>
       <c r="F221" t="n">
-        <v>370</v>
+        <v>457</v>
       </c>
     </row>
     <row r="222">
@@ -5609,13 +5609,13 @@
         <v>12.4578</v>
       </c>
       <c r="D222" t="n">
-        <v>1453.2647702407</v>
+        <v>1669.1316872428</v>
       </c>
       <c r="E222" t="n">
-        <v>1453.2647702407</v>
+        <v>1669.1316872428</v>
       </c>
       <c r="F222" t="n">
-        <v>664142</v>
+        <v>811198</v>
       </c>
     </row>
     <row r="223">
@@ -5629,13 +5629,13 @@
         <v>6.6131</v>
       </c>
       <c r="D223" t="n">
-        <v>842.606126914661</v>
+        <v>930.446502057613</v>
       </c>
       <c r="E223" t="n">
-        <v>842.606126914661</v>
+        <v>930.446502057613</v>
       </c>
       <c r="F223" t="n">
-        <v>385071</v>
+        <v>452197</v>
       </c>
     </row>
     <row r="224">
@@ -5649,13 +5649,13 @@
         <v>45.079162</v>
       </c>
       <c r="D224" t="n">
-        <v>234690.056892779</v>
+        <v>246005.495884774</v>
       </c>
       <c r="E224" t="n">
-        <v>234690.056892779</v>
+        <v>246005.495884774</v>
       </c>
       <c r="F224" t="n">
-        <v>107253356</v>
+        <v>119558671</v>
       </c>
     </row>
     <row r="225">
@@ -5669,13 +5669,13 @@
         <v>-14.4524</v>
       </c>
       <c r="D225" t="n">
-        <v>13976.9803063457</v>
+        <v>15563.7839506173</v>
       </c>
       <c r="E225" t="n">
-        <v>13976.9803063457</v>
+        <v>15563.7839506173</v>
       </c>
       <c r="F225" t="n">
-        <v>6387480</v>
+        <v>7563999</v>
       </c>
     </row>
     <row r="226">
@@ -5689,13 +5689,13 @@
         <v>21.0059</v>
       </c>
       <c r="D226" t="n">
-        <v>152636.343544858</v>
+        <v>185077.833333333</v>
       </c>
       <c r="E226" t="n">
-        <v>152636.343544858</v>
+        <v>185077.833333333</v>
       </c>
       <c r="F226" t="n">
-        <v>69754809</v>
+        <v>89947827</v>
       </c>
     </row>
     <row r="227">
@@ -5709,13 +5709,13 @@
         <v>55.492</v>
       </c>
       <c r="D227" t="n">
-        <v>685.540481400438</v>
+        <v>1076.15843621399</v>
       </c>
       <c r="E227" t="n">
-        <v>685.540481400438</v>
+        <v>1076.15843621399</v>
       </c>
       <c r="F227" t="n">
-        <v>313292</v>
+        <v>523013</v>
       </c>
     </row>
     <row r="228">
@@ -5729,13 +5729,13 @@
         <v>-11.779889</v>
       </c>
       <c r="D228" t="n">
-        <v>1875.56892778993</v>
+        <v>2006.85390946502</v>
       </c>
       <c r="E228" t="n">
-        <v>1875.56892778993</v>
+        <v>2006.85390946502</v>
       </c>
       <c r="F228" t="n">
-        <v>857135</v>
+        <v>975331</v>
       </c>
     </row>
     <row r="229">
@@ -5749,13 +5749,13 @@
         <v>103.8333</v>
       </c>
       <c r="D229" t="n">
-        <v>42019.2669584245</v>
+        <v>43171.5164609053</v>
       </c>
       <c r="E229" t="n">
-        <v>42019.2669584245</v>
+        <v>43171.5164609053</v>
       </c>
       <c r="F229" t="n">
-        <v>19202805</v>
+        <v>20981357</v>
       </c>
     </row>
     <row r="230">
@@ -5769,13 +5769,13 @@
         <v>19.699</v>
       </c>
       <c r="D230" t="n">
-        <v>90870.5557986871</v>
+        <v>108389.047325103</v>
       </c>
       <c r="E230" t="n">
-        <v>90870.5557986871</v>
+        <v>108389.047325103</v>
       </c>
       <c r="F230" t="n">
-        <v>41527844</v>
+        <v>52677077</v>
       </c>
     </row>
     <row r="231">
@@ -5789,13 +5789,13 @@
         <v>14.9955</v>
       </c>
       <c r="D231" t="n">
-        <v>57848.9190371991</v>
+        <v>68970.378600823</v>
       </c>
       <c r="E231" t="n">
-        <v>57848.9190371991</v>
+        <v>68970.378600823</v>
       </c>
       <c r="F231" t="n">
-        <v>26436956</v>
+        <v>33519604</v>
       </c>
     </row>
     <row r="232">
@@ -5809,13 +5809,13 @@
         <v>160.1562</v>
       </c>
       <c r="D232" t="n">
-        <v>6.73522975929978</v>
+        <v>7.52674897119342</v>
       </c>
       <c r="E232" t="n">
-        <v>6.73522975929978</v>
+        <v>7.52674897119342</v>
       </c>
       <c r="F232" t="n">
-        <v>3078</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="233">
@@ -5829,13 +5829,13 @@
         <v>46.199616</v>
       </c>
       <c r="D233" t="n">
-        <v>3682.54704595186</v>
+        <v>4310.0658436214</v>
       </c>
       <c r="E233" t="n">
-        <v>3682.54704595186</v>
+        <v>4310.0658436214</v>
       </c>
       <c r="F233" t="n">
-        <v>1682924</v>
+        <v>2094692</v>
       </c>
     </row>
     <row r="234">
@@ -5849,13 +5849,13 @@
         <v>22.9375</v>
       </c>
       <c r="D234" t="n">
-        <v>626975.035010941</v>
+        <v>684747.230452675</v>
       </c>
       <c r="E234" t="n">
-        <v>626975.035010941</v>
+        <v>684747.230452675</v>
       </c>
       <c r="F234" t="n">
-        <v>286527591</v>
+        <v>332787154</v>
       </c>
     </row>
     <row r="235">
@@ -5869,13 +5869,13 @@
         <v>31.307</v>
       </c>
       <c r="D235" t="n">
-        <v>2966.22757111597</v>
+        <v>3422.27572016461</v>
       </c>
       <c r="E235" t="n">
-        <v>2966.22757111597</v>
+        <v>3422.27572016461</v>
       </c>
       <c r="F235" t="n">
-        <v>1355566</v>
+        <v>1663226</v>
       </c>
     </row>
     <row r="236">
@@ -5889,13 +5889,13 @@
         <v>-3.74922</v>
       </c>
       <c r="D236" t="n">
-        <v>1130370.95185996</v>
+        <v>1275232.7345679</v>
       </c>
       <c r="E236" t="n">
-        <v>1130370.95185996</v>
+        <v>1275232.7345679</v>
       </c>
       <c r="F236" t="n">
-        <v>516579525</v>
+        <v>619763109</v>
       </c>
     </row>
     <row r="237">
@@ -5909,13 +5909,13 @@
         <v>80.771797</v>
       </c>
       <c r="D237" t="n">
-        <v>23446.7658643326</v>
+        <v>29440.4320987654</v>
       </c>
       <c r="E237" t="n">
-        <v>23446.7658643326</v>
+        <v>29440.4320987654</v>
       </c>
       <c r="F237" t="n">
-        <v>10715172</v>
+        <v>14308050</v>
       </c>
     </row>
     <row r="238">
@@ -5929,13 +5929,13 @@
         <v>30.2176</v>
       </c>
       <c r="D238" t="n">
-        <v>13907.5667396061</v>
+        <v>15128.6893004115</v>
       </c>
       <c r="E238" t="n">
-        <v>13907.5667396061</v>
+        <v>15128.6893004115</v>
       </c>
       <c r="F238" t="n">
-        <v>6355758</v>
+        <v>7352543</v>
       </c>
     </row>
     <row r="239">
@@ -5949,13 +5949,13 @@
         <v>-56.0278</v>
       </c>
       <c r="D239" t="n">
-        <v>3760.80306345733</v>
+        <v>4196.51851851852</v>
       </c>
       <c r="E239" t="n">
-        <v>3760.80306345733</v>
+        <v>4196.51851851852</v>
       </c>
       <c r="F239" t="n">
-        <v>1718687</v>
+        <v>2039508</v>
       </c>
     </row>
     <row r="240">
@@ -5969,13 +5969,13 @@
         <v>18.643501</v>
       </c>
       <c r="D240" t="n">
-        <v>229037.242888403</v>
+        <v>275010.479423868</v>
       </c>
       <c r="E240" t="n">
-        <v>229037.242888403</v>
+        <v>275010.479423868</v>
       </c>
       <c r="F240" t="n">
-        <v>104670020</v>
+        <v>133655093</v>
       </c>
     </row>
     <row r="241">
@@ -5989,13 +5989,13 @@
         <v>8.2275</v>
       </c>
       <c r="D241" t="n">
-        <v>199121.085339168</v>
+        <v>227122.102880658</v>
       </c>
       <c r="E241" t="n">
-        <v>199121.085339168</v>
+        <v>227122.102880658</v>
       </c>
       <c r="F241" t="n">
-        <v>90998336</v>
+        <v>110381342</v>
       </c>
     </row>
     <row r="242">
@@ -6009,13 +6009,13 @@
         <v>38.996815</v>
       </c>
       <c r="D242" t="n">
-        <v>5753.90153172866</v>
+        <v>6791.46502057613</v>
       </c>
       <c r="E242" t="n">
-        <v>5753.90153172866</v>
+        <v>6791.46502057613</v>
       </c>
       <c r="F242" t="n">
-        <v>2629533</v>
+        <v>3300652</v>
       </c>
     </row>
     <row r="243">
@@ -6029,13 +6029,13 @@
         <v>121</v>
       </c>
       <c r="D243" t="n">
-        <v>551.336980306346</v>
+        <v>603.681069958848</v>
       </c>
       <c r="E243" t="n">
-        <v>551.336980306346</v>
+        <v>603.681069958848</v>
       </c>
       <c r="F243" t="n">
-        <v>251961</v>
+        <v>293389</v>
       </c>
     </row>
     <row r="244">
@@ -6049,13 +6049,13 @@
         <v>71.2761</v>
       </c>
       <c r="D244" t="n">
-        <v>7649.55361050328</v>
+        <v>7987.1975308642</v>
       </c>
       <c r="E244" t="n">
-        <v>7649.55361050328</v>
+        <v>7987.1975308642</v>
       </c>
       <c r="F244" t="n">
-        <v>3495846</v>
+        <v>3881778</v>
       </c>
     </row>
     <row r="245">
@@ -6069,13 +6069,13 @@
         <v>34.888822</v>
       </c>
       <c r="D245" t="n">
-        <v>407.544857768053</v>
+        <v>413.598765432099</v>
       </c>
       <c r="E245" t="n">
-        <v>407.544857768053</v>
+        <v>413.598765432099</v>
       </c>
       <c r="F245" t="n">
-        <v>186248</v>
+        <v>201009</v>
       </c>
     </row>
     <row r="246">
@@ -6089,13 +6089,13 @@
         <v>100.992541</v>
       </c>
       <c r="D246" t="n">
-        <v>8006.79868708972</v>
+        <v>12419.6604938272</v>
       </c>
       <c r="E246" t="n">
-        <v>8006.79868708972</v>
+        <v>12419.6604938272</v>
       </c>
       <c r="F246" t="n">
-        <v>3659107</v>
+        <v>6035955</v>
       </c>
     </row>
     <row r="247">
@@ -6109,13 +6109,13 @@
         <v>125.727539</v>
       </c>
       <c r="D247" t="n">
-        <v>92.5929978118162</v>
+        <v>277.711934156379</v>
       </c>
       <c r="E247" t="n">
-        <v>92.5929978118162</v>
+        <v>277.711934156379</v>
       </c>
       <c r="F247" t="n">
-        <v>42315</v>
+        <v>134968</v>
       </c>
     </row>
     <row r="248">
@@ -6129,13 +6129,13 @@
         <v>0.8248</v>
       </c>
       <c r="D248" t="n">
-        <v>2636.12910284464</v>
+        <v>3259.68518518519</v>
       </c>
       <c r="E248" t="n">
-        <v>2636.12910284464</v>
+        <v>3259.68518518519</v>
       </c>
       <c r="F248" t="n">
-        <v>1204711</v>
+        <v>1584207</v>
       </c>
     </row>
     <row r="249">
@@ -6149,13 +6149,13 @@
         <v>-61.2225</v>
       </c>
       <c r="D249" t="n">
-        <v>3432.39387308534</v>
+        <v>4012.74691358025</v>
       </c>
       <c r="E249" t="n">
-        <v>3432.39387308534</v>
+        <v>4012.74691358025</v>
       </c>
       <c r="F249" t="n">
-        <v>1568604</v>
+        <v>1950195</v>
       </c>
     </row>
     <row r="250">
@@ -6169,13 +6169,13 @@
         <v>9.537499</v>
       </c>
       <c r="D250" t="n">
-        <v>71962.6126914661</v>
+        <v>86566.7777777778</v>
       </c>
       <c r="E250" t="n">
-        <v>71962.6126914661</v>
+        <v>86566.7777777778</v>
       </c>
       <c r="F250" t="n">
-        <v>32886914</v>
+        <v>42071454</v>
       </c>
     </row>
     <row r="251">
@@ -6189,13 +6189,13 @@
         <v>35.2433</v>
       </c>
       <c r="D251" t="n">
-        <v>949472.643326039</v>
+        <v>1187821.9218107</v>
       </c>
       <c r="E251" t="n">
-        <v>949472.643326039</v>
+        <v>1187821.9218107</v>
       </c>
       <c r="F251" t="n">
-        <v>433908998</v>
+        <v>577281454</v>
       </c>
     </row>
     <row r="252">
@@ -6209,13 +6209,13 @@
         <v>-100</v>
       </c>
       <c r="D252" t="n">
-        <v>10584080.0525164</v>
+        <v>11897742.6666667</v>
       </c>
       <c r="E252" t="n">
-        <v>10584080.0525164</v>
+        <v>11897742.6666667</v>
       </c>
       <c r="F252" t="n">
-        <v>4836924584</v>
+        <v>5782302936</v>
       </c>
     </row>
     <row r="253">
@@ -6229,13 +6229,13 @@
         <v>32.290275</v>
       </c>
       <c r="D253" t="n">
-        <v>14080.9956236324</v>
+        <v>15763.6543209877</v>
       </c>
       <c r="E253" t="n">
-        <v>14080.9956236324</v>
+        <v>15763.6543209877</v>
       </c>
       <c r="F253" t="n">
-        <v>6435015</v>
+        <v>7661136</v>
       </c>
     </row>
     <row r="254">
@@ -6249,13 +6249,13 @@
         <v>31.1656</v>
       </c>
       <c r="D254" t="n">
-        <v>504130.824945295</v>
+        <v>602749.283950617</v>
       </c>
       <c r="E254" t="n">
-        <v>504130.824945295</v>
+        <v>602749.283950617</v>
       </c>
       <c r="F254" t="n">
-        <v>230387787</v>
+        <v>292936152</v>
       </c>
     </row>
     <row r="255">
@@ -6269,13 +6269,13 @@
         <v>53.847818</v>
       </c>
       <c r="D255" t="n">
-        <v>139693.168490153</v>
+        <v>163075.606995885</v>
       </c>
       <c r="E255" t="n">
-        <v>139693.168490153</v>
+        <v>163075.606995885</v>
       </c>
       <c r="F255" t="n">
-        <v>63839778</v>
+        <v>79254745</v>
       </c>
     </row>
     <row r="256">
@@ -6289,13 +6289,13 @@
         <v>-63.0686</v>
       </c>
       <c r="D256" t="n">
-        <v>7.06345733041575</v>
+        <v>12.2777777777778</v>
       </c>
       <c r="E256" t="n">
-        <v>7.06345733041575</v>
+        <v>12.2777777777778</v>
       </c>
       <c r="F256" t="n">
-        <v>3228</v>
+        <v>5967</v>
       </c>
     </row>
     <row r="257">
@@ -6309,13 +6309,13 @@
         <v>-64.7505</v>
       </c>
       <c r="D257" t="n">
-        <v>342.754923413567</v>
+        <v>466.718106995885</v>
       </c>
       <c r="E257" t="n">
-        <v>342.754923413567</v>
+        <v>466.718106995885</v>
       </c>
       <c r="F257" t="n">
-        <v>156639</v>
+        <v>226825</v>
       </c>
     </row>
     <row r="258">
@@ -6329,13 +6329,13 @@
         <v>-64.64</v>
       </c>
       <c r="D258" t="n">
-        <v>55.6695842450766</v>
+        <v>65.2757201646091</v>
       </c>
       <c r="E258" t="n">
-        <v>55.6695842450766</v>
+        <v>65.2757201646091</v>
       </c>
       <c r="F258" t="n">
-        <v>25441</v>
+        <v>31724</v>
       </c>
     </row>
     <row r="259">
@@ -6349,13 +6349,13 @@
         <v>-81.2546</v>
       </c>
       <c r="D259" t="n">
-        <v>224.494529540481</v>
+        <v>243.960905349794</v>
       </c>
       <c r="E259" t="n">
-        <v>224.494529540481</v>
+        <v>243.960905349794</v>
       </c>
       <c r="F259" t="n">
-        <v>102594</v>
+        <v>118565</v>
       </c>
     </row>
     <row r="260">
@@ -6369,13 +6369,13 @@
         <v>-2.3644</v>
       </c>
       <c r="D260" t="n">
-        <v>1439.2932166302</v>
+        <v>1596.0329218107</v>
       </c>
       <c r="E260" t="n">
-        <v>1439.2932166302</v>
+        <v>1596.0329218107</v>
       </c>
       <c r="F260" t="n">
-        <v>657757</v>
+        <v>775672</v>
       </c>
     </row>
     <row r="261">
@@ -6389,13 +6389,13 @@
         <v>-59.5236</v>
       </c>
       <c r="D261" t="n">
-        <v>20.1006564551422</v>
+        <v>22.6604938271605</v>
       </c>
       <c r="E261" t="n">
-        <v>20.1006564551422</v>
+        <v>22.6604938271605</v>
       </c>
       <c r="F261" t="n">
-        <v>9186</v>
+        <v>11013</v>
       </c>
     </row>
     <row r="262">
@@ -6409,13 +6409,13 @@
         <v>-5.3536</v>
       </c>
       <c r="D262" t="n">
-        <v>1249.70897155361</v>
+        <v>1430.81893004115</v>
       </c>
       <c r="E262" t="n">
-        <v>1249.70897155361</v>
+        <v>1430.81893004115</v>
       </c>
       <c r="F262" t="n">
-        <v>571117</v>
+        <v>695378</v>
       </c>
     </row>
     <row r="263">
@@ -6429,13 +6429,13 @@
         <v>-4.5481</v>
       </c>
       <c r="D263" t="n">
-        <v>413.35010940919</v>
+        <v>483.510288065844</v>
       </c>
       <c r="E263" t="n">
-        <v>413.35010940919</v>
+        <v>483.510288065844</v>
       </c>
       <c r="F263" t="n">
-        <v>188901</v>
+        <v>234986</v>
       </c>
     </row>
     <row r="264">
@@ -6449,13 +6449,13 @@
         <v>-62.187366</v>
       </c>
       <c r="D264" t="n">
-        <v>11.6323851203501</v>
+        <v>12.1316872427984</v>
       </c>
       <c r="E264" t="n">
-        <v>11.6323851203501</v>
+        <v>12.1316872427984</v>
       </c>
       <c r="F264" t="n">
-        <v>5316</v>
+        <v>5896</v>
       </c>
     </row>
     <row r="265">
@@ -6469,13 +6469,13 @@
         <v>-14.3559</v>
       </c>
       <c r="D265" t="n">
-        <v>1.61487964989059</v>
+        <v>1.75720164609054</v>
       </c>
       <c r="E265" t="n">
-        <v>1.61487964989059</v>
+        <v>1.75720164609054</v>
       </c>
       <c r="F265" t="n">
-        <v>738</v>
+        <v>854</v>
       </c>
     </row>
     <row r="266">
@@ -6489,13 +6489,13 @@
         <v>-71.7979</v>
       </c>
       <c r="D266" t="n">
-        <v>672.586433260394</v>
+        <v>775.399176954733</v>
       </c>
       <c r="E266" t="n">
-        <v>672.586433260394</v>
+        <v>775.399176954733</v>
       </c>
       <c r="F266" t="n">
-        <v>307372</v>
+        <v>376844</v>
       </c>
     </row>
     <row r="267">
@@ -6509,13 +6509,13 @@
         <v>-3.436</v>
       </c>
       <c r="D267" t="n">
-        <v>1348587.92560175</v>
+        <v>1532489.1563786</v>
       </c>
       <c r="E267" t="n">
-        <v>1348587.92560175</v>
+        <v>1532489.1563786</v>
       </c>
       <c r="F267" t="n">
-        <v>616304682</v>
+        <v>744789730</v>
       </c>
     </row>
     <row r="268">
@@ -6529,13 +6529,13 @@
         <v>-55.7658</v>
       </c>
       <c r="D268" t="n">
-        <v>18906.8380743982</v>
+        <v>30696.487654321</v>
       </c>
       <c r="E268" t="n">
-        <v>18906.8380743982</v>
+        <v>30696.487654321</v>
       </c>
       <c r="F268" t="n">
-        <v>8640425</v>
+        <v>14918493</v>
       </c>
     </row>
     <row r="269">
@@ -6549,13 +6549,13 @@
         <v>64.585262</v>
       </c>
       <c r="D269" t="n">
-        <v>40935.2625820569</v>
+        <v>44065.0576131687</v>
       </c>
       <c r="E269" t="n">
-        <v>40935.2625820569</v>
+        <v>44065.0576131687</v>
       </c>
       <c r="F269" t="n">
-        <v>18707415</v>
+        <v>21415618</v>
       </c>
     </row>
     <row r="270">
@@ -6569,13 +6569,13 @@
         <v>166.9592</v>
       </c>
       <c r="D270" t="n">
-        <v>0.564551422319475</v>
+        <v>0.769547325102881</v>
       </c>
       <c r="E270" t="n">
-        <v>0.564551422319475</v>
+        <v>0.769547325102881</v>
       </c>
       <c r="F270" t="n">
-        <v>258</v>
+        <v>374</v>
       </c>
     </row>
     <row r="271">
@@ -6589,13 +6589,13 @@
         <v>-66.5897</v>
       </c>
       <c r="D271" t="n">
-        <v>61689.7592997812</v>
+        <v>70254.9238683128</v>
       </c>
       <c r="E271" t="n">
-        <v>61689.7592997812</v>
+        <v>70254.9238683128</v>
       </c>
       <c r="F271" t="n">
-        <v>28192220</v>
+        <v>34143893</v>
       </c>
     </row>
     <row r="272">
@@ -6609,13 +6609,13 @@
         <v>108.277199</v>
       </c>
       <c r="D272" t="n">
-        <v>1023.75054704595</v>
+        <v>1169.77160493827</v>
       </c>
       <c r="E272" t="n">
-        <v>1023.75054704595</v>
+        <v>1169.77160493827</v>
       </c>
       <c r="F272" t="n">
-        <v>467854</v>
+        <v>568509</v>
       </c>
     </row>
     <row r="273">
@@ -6629,13 +6629,13 @@
         <v>35.2332</v>
       </c>
       <c r="D273" t="n">
-        <v>67144.3435448578</v>
+        <v>81002.9403292181</v>
       </c>
       <c r="E273" t="n">
-        <v>67144.3435448578</v>
+        <v>81002.9403292181</v>
       </c>
       <c r="F273" t="n">
-        <v>30684965</v>
+        <v>39367429</v>
       </c>
     </row>
     <row r="274">
@@ -6649,13 +6649,13 @@
         <v>48.516388</v>
       </c>
       <c r="D274" t="n">
-        <v>1581.59080962801</v>
+        <v>1869.52469135802</v>
       </c>
       <c r="E274" t="n">
-        <v>1581.59080962801</v>
+        <v>1869.52469135802</v>
       </c>
       <c r="F274" t="n">
-        <v>722787</v>
+        <v>908589</v>
       </c>
     </row>
     <row r="275">
@@ -6669,13 +6669,13 @@
         <v>27.849332</v>
       </c>
       <c r="D275" t="n">
-        <v>22049.8905908096</v>
+        <v>26222.6008230453</v>
       </c>
       <c r="E275" t="n">
-        <v>22049.8905908096</v>
+        <v>26222.6008230453</v>
       </c>
       <c r="F275" t="n">
-        <v>10076800</v>
+        <v>12744184</v>
       </c>
     </row>
     <row r="276">
@@ -6689,13 +6689,13 @@
         <v>29.154857</v>
       </c>
       <c r="D276" t="n">
-        <v>11075.3457330416</v>
+        <v>12704.3086419753</v>
       </c>
       <c r="E276" t="n">
-        <v>11075.3457330416</v>
+        <v>12704.3086419753</v>
       </c>
       <c r="F276" t="n">
-        <v>5061433</v>
+        <v>6174294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>